<commit_message>
by saw lay -Group creation
</commit_message>
<xml_diff>
--- a/DataSource/InputData.xlsx
+++ b/DataSource/InputData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Syntegrate\source\repos\DEV_3_Nevron_1205\DataSource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A322C082-11B0-4CB9-855A-75C14321C6E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FDFFA9F-2DAF-4927-9698-A11D678CA8E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-1530" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="180">
   <si>
     <t>A</t>
   </si>
@@ -776,6 +776,9 @@
   </si>
   <si>
     <t>Brown</t>
+  </si>
+  <si>
+    <t>Group color</t>
   </si>
 </sst>
 </file>
@@ -1273,7 +1276,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1406,15 +1409,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1430,20 +1451,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2603,13 +2618,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:P60"/>
+  <dimension ref="A1:Q60"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="3" topLeftCell="E15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G35" sqref="G35"/>
+      <selection pane="bottomRight" activeCell="E62" sqref="E62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="20.100000000000001" customHeight="1"/>
@@ -2617,2065 +2632,2334 @@
     <col min="1" max="1" width="6.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="16.85546875" style="43" customWidth="1"/>
     <col min="3" max="3" width="12" style="1" customWidth="1"/>
-    <col min="4" max="4" width="20" style="1" customWidth="1"/>
-    <col min="5" max="5" width="6.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12" style="1" customWidth="1"/>
-    <col min="7" max="7" width="20" style="1" customWidth="1"/>
-    <col min="8" max="16" width="16.28515625" style="1" customWidth="1"/>
-    <col min="17" max="16384" width="16.28515625" style="1"/>
+    <col min="4" max="5" width="20" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12" style="1" customWidth="1"/>
+    <col min="8" max="8" width="20" style="1" customWidth="1"/>
+    <col min="9" max="17" width="16.28515625" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="16.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="27.6" customHeight="1">
-      <c r="A1" s="52" t="s">
+    <row r="1" spans="1:17" ht="27.6" customHeight="1">
+      <c r="A1" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
-      <c r="J1" s="52"/>
-      <c r="K1" s="52"/>
-      <c r="L1" s="52"/>
-      <c r="M1" s="52"/>
-      <c r="N1" s="52"/>
-      <c r="O1" s="52"/>
-      <c r="P1" s="52"/>
-    </row>
-    <row r="2" spans="1:16" ht="24" customHeight="1">
-      <c r="A2" s="50"/>
-      <c r="B2" s="50"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50"/>
-      <c r="I2" s="50"/>
-      <c r="J2" s="50"/>
-      <c r="K2" s="50"/>
-      <c r="L2" s="50"/>
-      <c r="M2" s="51"/>
-      <c r="N2" s="47"/>
-      <c r="O2" s="48"/>
-      <c r="P2" s="49"/>
-    </row>
-    <row r="3" spans="1:16" ht="20.25" customHeight="1" thickBot="1">
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
+      <c r="N1" s="46"/>
+      <c r="O1" s="46"/>
+      <c r="P1" s="46"/>
+      <c r="Q1" s="46"/>
+    </row>
+    <row r="2" spans="1:17" ht="24" customHeight="1">
+      <c r="A2" s="56"/>
+      <c r="B2" s="56"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="56"/>
+      <c r="J2" s="56"/>
+      <c r="K2" s="56"/>
+      <c r="L2" s="56"/>
+      <c r="M2" s="56"/>
+      <c r="N2" s="57"/>
+      <c r="O2" s="53"/>
+      <c r="P2" s="54"/>
+      <c r="Q2" s="55"/>
+    </row>
+    <row r="3" spans="1:17" ht="20.25" customHeight="1" thickBot="1">
       <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="53" t="s">
+      <c r="C3" s="47" t="s">
         <v>149</v>
       </c>
-      <c r="D3" s="53"/>
-      <c r="E3" s="7" t="s">
+      <c r="D3" s="47"/>
+      <c r="E3" s="59" t="s">
+        <v>179</v>
+      </c>
+      <c r="F3" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="G3" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="H3" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="I3" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="J3" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="J3" s="8" t="s">
+      <c r="K3" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="K3" s="8" t="s">
+      <c r="L3" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="L3" s="9" t="s">
+      <c r="M3" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="M3" s="36" t="s">
+      <c r="N3" s="36" t="s">
         <v>172</v>
       </c>
-      <c r="N3" s="10" t="s">
+      <c r="O3" s="10" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="20.25" customHeight="1" thickTop="1">
+    <row r="4" spans="1:17" ht="20.25" customHeight="1" thickTop="1">
       <c r="A4" s="3">
         <v>1</v>
       </c>
       <c r="B4" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="C4" s="54" t="s">
+      <c r="C4" s="48" t="s">
         <v>87</v>
       </c>
-      <c r="D4" s="44" t="s">
+      <c r="D4" s="60" t="s">
         <v>91</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E4" s="44" t="s">
+        <v>173</v>
+      </c>
+      <c r="F4" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="G4" s="15" t="s">
+      <c r="G4" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="H4" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="H4" s="24">
+      <c r="I4" s="24">
         <v>805.12</v>
       </c>
-      <c r="I4" s="16"/>
       <c r="J4" s="16"/>
-      <c r="K4" s="16">
-        <v>4800</v>
-      </c>
+      <c r="K4" s="16"/>
       <c r="L4" s="16">
+        <v>4800</v>
+      </c>
+      <c r="M4" s="16">
         <v>1</v>
       </c>
-      <c r="M4" s="37"/>
-      <c r="N4" s="17" t="s">
+      <c r="N4" s="37"/>
+      <c r="O4" s="17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="20.100000000000001" customHeight="1">
+    <row r="5" spans="1:17" ht="20.100000000000001" customHeight="1">
       <c r="A5" s="3">
         <v>2</v>
       </c>
       <c r="B5" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="C5" s="55"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="18" t="s">
+      <c r="C5" s="49"/>
+      <c r="D5" s="60" t="s">
+        <v>91</v>
+      </c>
+      <c r="E5" s="44" t="s">
+        <v>173</v>
+      </c>
+      <c r="F5" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="G5" s="20" t="s">
+      <c r="G5" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="H5" s="20" t="s">
         <v>176</v>
       </c>
-      <c r="H5" s="25">
+      <c r="I5" s="25">
         <v>3983.44</v>
       </c>
-      <c r="I5" s="21"/>
       <c r="J5" s="21"/>
-      <c r="K5" s="16">
-        <v>4800</v>
-      </c>
-      <c r="L5" s="21">
+      <c r="K5" s="21"/>
+      <c r="L5" s="16">
+        <v>4800</v>
+      </c>
+      <c r="M5" s="21">
         <v>1</v>
       </c>
-      <c r="M5" s="38"/>
-      <c r="N5" s="17" t="s">
+      <c r="N5" s="38"/>
+      <c r="O5" s="17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="20.100000000000001" customHeight="1">
+    <row r="6" spans="1:17" ht="20.100000000000001" customHeight="1">
       <c r="A6" s="3">
         <v>3</v>
       </c>
       <c r="B6" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="C6" s="55"/>
-      <c r="D6" s="44" t="s">
+      <c r="C6" s="49"/>
+      <c r="D6" s="60" t="s">
         <v>90</v>
       </c>
-      <c r="E6" s="18" t="s">
+      <c r="E6" s="44" t="s">
+        <v>177</v>
+      </c>
+      <c r="F6" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="G6" s="20" t="s">
+      <c r="G6" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="H6" s="20" t="s">
         <v>153</v>
       </c>
-      <c r="H6" s="25">
+      <c r="I6" s="25">
         <v>5615.03</v>
       </c>
-      <c r="I6" s="21"/>
       <c r="J6" s="21"/>
-      <c r="K6" s="16">
-        <v>4800</v>
-      </c>
-      <c r="L6" s="21">
+      <c r="K6" s="21"/>
+      <c r="L6" s="16">
+        <v>4800</v>
+      </c>
+      <c r="M6" s="21">
         <v>1</v>
       </c>
-      <c r="M6" s="38"/>
-      <c r="N6" s="17" t="s">
+      <c r="N6" s="38"/>
+      <c r="O6" s="17" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="20.85" customHeight="1">
+    <row r="7" spans="1:17" ht="20.85" customHeight="1">
       <c r="A7" s="4">
         <v>4</v>
       </c>
       <c r="B7" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="C7" s="55"/>
-      <c r="D7" s="45"/>
-      <c r="E7" s="18" t="s">
+      <c r="C7" s="49"/>
+      <c r="D7" s="60" t="s">
+        <v>90</v>
+      </c>
+      <c r="E7" s="44" t="s">
+        <v>177</v>
+      </c>
+      <c r="F7" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="G7" s="20" t="s">
+      <c r="G7" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="H7" s="20" t="s">
         <v>154</v>
       </c>
-      <c r="H7" s="25">
+      <c r="I7" s="25">
         <v>1885.68</v>
       </c>
-      <c r="I7" s="21"/>
       <c r="J7" s="21"/>
-      <c r="K7" s="16">
-        <v>4800</v>
-      </c>
-      <c r="L7" s="21">
+      <c r="K7" s="21"/>
+      <c r="L7" s="16">
+        <v>4800</v>
+      </c>
+      <c r="M7" s="21">
         <v>1</v>
       </c>
-      <c r="M7" s="38"/>
-      <c r="N7" s="17" t="s">
+      <c r="N7" s="38"/>
+      <c r="O7" s="17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="20.100000000000001" customHeight="1">
+    <row r="8" spans="1:17" ht="20.100000000000001" customHeight="1">
       <c r="A8" s="4">
         <v>5</v>
       </c>
       <c r="B8" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="C8" s="55"/>
-      <c r="D8" s="45"/>
-      <c r="E8" s="18" t="s">
+      <c r="C8" s="49"/>
+      <c r="D8" s="60" t="s">
+        <v>90</v>
+      </c>
+      <c r="E8" s="44" t="s">
+        <v>177</v>
+      </c>
+      <c r="F8" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="G8" s="20" t="s">
+      <c r="G8" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="H8" s="20" t="s">
         <v>173</v>
       </c>
-      <c r="H8" s="25">
+      <c r="I8" s="25">
         <v>2495.8000000000002</v>
       </c>
-      <c r="I8" s="21"/>
       <c r="J8" s="21"/>
-      <c r="K8" s="16">
-        <v>4800</v>
-      </c>
-      <c r="L8" s="21">
+      <c r="K8" s="21"/>
+      <c r="L8" s="16">
+        <v>4800</v>
+      </c>
+      <c r="M8" s="21">
         <v>1</v>
       </c>
-      <c r="M8" s="38"/>
-      <c r="N8" s="17" t="s">
+      <c r="N8" s="38"/>
+      <c r="O8" s="17" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="20.100000000000001" customHeight="1">
+    <row r="9" spans="1:17" ht="20.100000000000001" customHeight="1">
       <c r="A9" s="3">
         <v>6</v>
       </c>
       <c r="B9" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="C9" s="55"/>
-      <c r="D9" s="46"/>
-      <c r="E9" s="18" t="s">
+      <c r="C9" s="49"/>
+      <c r="D9" s="60" t="s">
+        <v>90</v>
+      </c>
+      <c r="E9" s="44" t="s">
+        <v>177</v>
+      </c>
+      <c r="F9" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="19" t="s">
+      <c r="G9" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="G9" s="20" t="s">
+      <c r="H9" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="H9" s="26">
+      <c r="I9" s="26">
         <v>475.39</v>
       </c>
-      <c r="I9" s="21"/>
       <c r="J9" s="21"/>
-      <c r="K9" s="16">
-        <v>4800</v>
-      </c>
-      <c r="L9" s="21">
+      <c r="K9" s="21"/>
+      <c r="L9" s="16">
+        <v>4800</v>
+      </c>
+      <c r="M9" s="21">
         <v>2</v>
       </c>
-      <c r="M9" s="38"/>
-      <c r="N9" s="17" t="s">
+      <c r="N9" s="38"/>
+      <c r="O9" s="17" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="20.100000000000001" customHeight="1">
+    <row r="10" spans="1:17" ht="20.100000000000001" customHeight="1">
       <c r="A10" s="3">
         <v>7</v>
       </c>
       <c r="B10" s="23" t="s">
         <v>74</v>
       </c>
-      <c r="C10" s="55"/>
-      <c r="D10" s="44" t="s">
+      <c r="C10" s="49"/>
+      <c r="D10" s="60" t="s">
         <v>89</v>
       </c>
-      <c r="E10" s="18" t="s">
+      <c r="E10" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="F10" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="F10" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="G10" s="20" t="s">
+      <c r="G10" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="H10" s="20" t="s">
         <v>174</v>
       </c>
-      <c r="H10" s="25">
+      <c r="I10" s="25">
         <v>7368</v>
       </c>
-      <c r="I10" s="21"/>
       <c r="J10" s="21"/>
-      <c r="K10" s="16">
-        <v>4800</v>
-      </c>
-      <c r="L10" s="21">
+      <c r="K10" s="21"/>
+      <c r="L10" s="16">
+        <v>4800</v>
+      </c>
+      <c r="M10" s="21">
         <v>2</v>
       </c>
-      <c r="M10" s="38"/>
-      <c r="N10" s="17" t="s">
+      <c r="N10" s="38"/>
+      <c r="O10" s="17" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="20.100000000000001" customHeight="1">
+    <row r="11" spans="1:17" ht="20.100000000000001" customHeight="1">
       <c r="A11" s="3">
         <v>8</v>
       </c>
       <c r="B11" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="C11" s="55"/>
-      <c r="D11" s="46"/>
-      <c r="E11" s="18" t="s">
+      <c r="C11" s="49"/>
+      <c r="D11" s="60" t="s">
+        <v>89</v>
+      </c>
+      <c r="E11" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="F11" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="F11" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="G11" s="20" t="s">
+      <c r="G11" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="H11" s="20" t="s">
         <v>175</v>
       </c>
-      <c r="H11" s="25">
+      <c r="I11" s="25">
         <v>1499.07</v>
       </c>
-      <c r="I11" s="21"/>
       <c r="J11" s="21"/>
-      <c r="K11" s="16">
-        <v>4800</v>
-      </c>
-      <c r="L11" s="21">
+      <c r="K11" s="21"/>
+      <c r="L11" s="16">
+        <v>4800</v>
+      </c>
+      <c r="M11" s="21">
         <v>2</v>
       </c>
-      <c r="M11" s="38"/>
-      <c r="N11" s="17" t="s">
+      <c r="N11" s="38"/>
+      <c r="O11" s="17" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="20.100000000000001" customHeight="1">
+    <row r="12" spans="1:17" ht="20.100000000000001" customHeight="1">
       <c r="A12" s="3">
         <v>9</v>
       </c>
       <c r="B12" s="23" t="s">
         <v>76</v>
       </c>
-      <c r="C12" s="55"/>
-      <c r="D12" s="44" t="s">
+      <c r="C12" s="49"/>
+      <c r="D12" s="60" t="s">
         <v>88</v>
       </c>
-      <c r="E12" s="18" t="s">
+      <c r="E12" s="44" t="s">
+        <v>154</v>
+      </c>
+      <c r="F12" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="G12" s="20" t="s">
+      <c r="G12" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="H12" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="H12" s="26">
+      <c r="I12" s="26">
         <v>322.32</v>
       </c>
-      <c r="I12" s="21"/>
       <c r="J12" s="21"/>
-      <c r="K12" s="16">
-        <v>4800</v>
-      </c>
-      <c r="L12" s="21">
+      <c r="K12" s="21"/>
+      <c r="L12" s="16">
+        <v>4800</v>
+      </c>
+      <c r="M12" s="21">
         <v>2</v>
       </c>
-      <c r="M12" s="38"/>
-      <c r="N12" s="17" t="s">
+      <c r="N12" s="38"/>
+      <c r="O12" s="17" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="20.100000000000001" customHeight="1">
+    <row r="13" spans="1:17" ht="20.100000000000001" customHeight="1">
       <c r="A13" s="3">
         <v>10</v>
       </c>
       <c r="B13" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="C13" s="55"/>
-      <c r="D13" s="45"/>
-      <c r="E13" s="18" t="s">
+      <c r="C13" s="49"/>
+      <c r="D13" s="60" t="s">
+        <v>88</v>
+      </c>
+      <c r="E13" s="44" t="s">
+        <v>154</v>
+      </c>
+      <c r="F13" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="F13" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="G13" s="20" t="s">
+      <c r="G13" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="H13" s="20" t="s">
         <v>153</v>
       </c>
-      <c r="H13" s="26">
+      <c r="I13" s="26">
         <v>479.52</v>
       </c>
-      <c r="I13" s="21"/>
       <c r="J13" s="21"/>
-      <c r="K13" s="16">
-        <v>4800</v>
-      </c>
-      <c r="L13" s="21">
-        <v>3</v>
-      </c>
-      <c r="M13" s="38"/>
-      <c r="N13" s="17" t="s">
+      <c r="K13" s="21"/>
+      <c r="L13" s="16">
+        <v>4800</v>
+      </c>
+      <c r="M13" s="21">
+        <v>3</v>
+      </c>
+      <c r="N13" s="38"/>
+      <c r="O13" s="17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="20.100000000000001" customHeight="1">
+    <row r="14" spans="1:17" ht="20.100000000000001" customHeight="1">
       <c r="A14" s="3">
         <v>11</v>
       </c>
       <c r="B14" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="C14" s="55"/>
-      <c r="D14" s="45"/>
-      <c r="E14" s="18" t="s">
+      <c r="C14" s="49"/>
+      <c r="D14" s="60" t="s">
+        <v>88</v>
+      </c>
+      <c r="E14" s="44" t="s">
+        <v>154</v>
+      </c>
+      <c r="F14" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="F14" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="G14" s="20" t="s">
+      <c r="G14" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="H14" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="H14" s="26">
+      <c r="I14" s="26">
         <v>195.84</v>
       </c>
-      <c r="I14" s="21"/>
       <c r="J14" s="21"/>
-      <c r="K14" s="16">
-        <v>4800</v>
-      </c>
-      <c r="L14" s="21">
-        <v>3</v>
-      </c>
-      <c r="M14" s="38"/>
-      <c r="N14" s="17" t="s">
+      <c r="K14" s="21"/>
+      <c r="L14" s="16">
+        <v>4800</v>
+      </c>
+      <c r="M14" s="21">
+        <v>3</v>
+      </c>
+      <c r="N14" s="38"/>
+      <c r="O14" s="17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="20.100000000000001" customHeight="1">
+    <row r="15" spans="1:17" ht="20.100000000000001" customHeight="1">
       <c r="A15" s="3">
         <v>12</v>
       </c>
       <c r="B15" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="C15" s="55"/>
-      <c r="D15" s="45"/>
-      <c r="E15" s="18" t="s">
+      <c r="C15" s="49"/>
+      <c r="D15" s="60" t="s">
+        <v>88</v>
+      </c>
+      <c r="E15" s="44" t="s">
+        <v>154</v>
+      </c>
+      <c r="F15" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="F15" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="G15" s="20" t="s">
+      <c r="G15" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="H15" s="20" t="s">
         <v>173</v>
       </c>
-      <c r="H15" s="26">
+      <c r="I15" s="26">
         <v>139.12</v>
       </c>
-      <c r="I15" s="21"/>
       <c r="J15" s="21"/>
-      <c r="K15" s="16">
-        <v>4800</v>
-      </c>
-      <c r="L15" s="21">
-        <v>3</v>
-      </c>
-      <c r="M15" s="38"/>
-      <c r="N15" s="17" t="s">
+      <c r="K15" s="21"/>
+      <c r="L15" s="16">
+        <v>4800</v>
+      </c>
+      <c r="M15" s="21">
+        <v>3</v>
+      </c>
+      <c r="N15" s="38"/>
+      <c r="O15" s="17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="20.100000000000001" customHeight="1">
+    <row r="16" spans="1:17" ht="20.100000000000001" customHeight="1">
       <c r="A16" s="3">
         <v>13</v>
       </c>
       <c r="B16" s="23" t="s">
         <v>80</v>
       </c>
-      <c r="C16" s="55"/>
-      <c r="D16" s="45"/>
-      <c r="E16" s="18" t="s">
+      <c r="C16" s="49"/>
+      <c r="D16" s="60" t="s">
+        <v>88</v>
+      </c>
+      <c r="E16" s="44" t="s">
+        <v>154</v>
+      </c>
+      <c r="F16" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="F16" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="G16" s="20" t="s">
+      <c r="G16" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="H16" s="20" t="s">
         <v>178</v>
       </c>
-      <c r="H16" s="26">
+      <c r="I16" s="26">
         <v>391.68</v>
       </c>
-      <c r="I16" s="21"/>
       <c r="J16" s="21"/>
-      <c r="K16" s="16">
-        <v>4800</v>
-      </c>
-      <c r="L16" s="21">
-        <v>3</v>
-      </c>
-      <c r="M16" s="38"/>
-      <c r="N16" s="17" t="s">
+      <c r="K16" s="21"/>
+      <c r="L16" s="16">
+        <v>4800</v>
+      </c>
+      <c r="M16" s="21">
+        <v>3</v>
+      </c>
+      <c r="N16" s="38"/>
+      <c r="O16" s="17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="20.100000000000001" customHeight="1">
+    <row r="17" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A17" s="3">
         <v>14</v>
       </c>
       <c r="B17" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="C17" s="55"/>
-      <c r="D17" s="45"/>
-      <c r="E17" s="18" t="s">
+      <c r="C17" s="49"/>
+      <c r="D17" s="60" t="s">
+        <v>88</v>
+      </c>
+      <c r="E17" s="44" t="s">
+        <v>154</v>
+      </c>
+      <c r="F17" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="F17" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="G17" s="20" t="s">
+      <c r="G17" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="H17" s="20" t="s">
         <v>174</v>
       </c>
-      <c r="H17" s="26">
+      <c r="I17" s="26">
         <v>97.92</v>
       </c>
-      <c r="I17" s="21"/>
       <c r="J17" s="21"/>
-      <c r="K17" s="16">
-        <v>4800</v>
-      </c>
-      <c r="L17" s="21">
-        <v>3</v>
-      </c>
-      <c r="M17" s="38"/>
-      <c r="N17" s="17" t="s">
+      <c r="K17" s="21"/>
+      <c r="L17" s="16">
+        <v>4800</v>
+      </c>
+      <c r="M17" s="21">
+        <v>3</v>
+      </c>
+      <c r="N17" s="38"/>
+      <c r="O17" s="17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="20.100000000000001" customHeight="1">
+    <row r="18" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A18" s="3">
         <v>15</v>
       </c>
       <c r="B18" s="23" t="s">
         <v>82</v>
       </c>
-      <c r="C18" s="55"/>
-      <c r="D18" s="45"/>
-      <c r="E18" s="18" t="s">
+      <c r="C18" s="49"/>
+      <c r="D18" s="60" t="s">
+        <v>88</v>
+      </c>
+      <c r="E18" s="44" t="s">
+        <v>154</v>
+      </c>
+      <c r="F18" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="F18" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="G18" s="20" t="s">
+      <c r="G18" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="H18" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="H18" s="26">
+      <c r="I18" s="26">
         <v>391.68</v>
       </c>
-      <c r="I18" s="21"/>
       <c r="J18" s="21"/>
-      <c r="K18" s="16">
-        <v>4800</v>
-      </c>
-      <c r="L18" s="21">
-        <v>3</v>
-      </c>
-      <c r="M18" s="38"/>
-      <c r="N18" s="17" t="s">
+      <c r="K18" s="21"/>
+      <c r="L18" s="16">
+        <v>4800</v>
+      </c>
+      <c r="M18" s="21">
+        <v>3</v>
+      </c>
+      <c r="N18" s="38"/>
+      <c r="O18" s="17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="20.100000000000001" customHeight="1">
+    <row r="19" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A19" s="3">
         <v>16</v>
       </c>
       <c r="B19" s="23" t="s">
         <v>83</v>
       </c>
-      <c r="C19" s="55"/>
-      <c r="D19" s="45"/>
-      <c r="E19" s="18" t="s">
+      <c r="C19" s="49"/>
+      <c r="D19" s="60" t="s">
+        <v>88</v>
+      </c>
+      <c r="E19" s="44" t="s">
+        <v>154</v>
+      </c>
+      <c r="F19" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="F19" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="G19" s="20" t="s">
+      <c r="G19" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="H19" s="20" t="s">
         <v>154</v>
       </c>
-      <c r="H19" s="26">
+      <c r="I19" s="26">
         <v>781.21</v>
       </c>
-      <c r="I19" s="21"/>
       <c r="J19" s="21"/>
-      <c r="K19" s="16">
-        <v>4800</v>
-      </c>
-      <c r="L19" s="21">
-        <v>3</v>
-      </c>
-      <c r="M19" s="38"/>
-      <c r="N19" s="17" t="s">
+      <c r="K19" s="21"/>
+      <c r="L19" s="16">
+        <v>4800</v>
+      </c>
+      <c r="M19" s="21">
+        <v>3</v>
+      </c>
+      <c r="N19" s="38"/>
+      <c r="O19" s="17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="20.100000000000001" customHeight="1">
+    <row r="20" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A20" s="3">
         <v>17</v>
       </c>
       <c r="B20" s="23" t="s">
         <v>84</v>
       </c>
-      <c r="C20" s="55"/>
-      <c r="D20" s="45"/>
-      <c r="E20" s="18" t="s">
+      <c r="C20" s="49"/>
+      <c r="D20" s="60" t="s">
+        <v>88</v>
+      </c>
+      <c r="E20" s="44" t="s">
+        <v>154</v>
+      </c>
+      <c r="F20" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="F20" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="G20" s="20" t="s">
+      <c r="G20" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="H20" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="H20" s="26">
+      <c r="I20" s="26">
         <v>541.44000000000005</v>
       </c>
-      <c r="I20" s="21"/>
       <c r="J20" s="21"/>
-      <c r="K20" s="16">
-        <v>4800</v>
-      </c>
-      <c r="L20" s="21">
-        <v>3</v>
-      </c>
-      <c r="M20" s="38"/>
-      <c r="N20" s="17" t="s">
+      <c r="K20" s="21"/>
+      <c r="L20" s="16">
+        <v>4800</v>
+      </c>
+      <c r="M20" s="21">
+        <v>3</v>
+      </c>
+      <c r="N20" s="38"/>
+      <c r="O20" s="17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="20.100000000000001" customHeight="1">
+    <row r="21" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A21" s="3">
         <v>18</v>
       </c>
       <c r="B21" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="C21" s="55"/>
-      <c r="D21" s="45"/>
-      <c r="E21" s="18" t="s">
+      <c r="C21" s="49"/>
+      <c r="D21" s="60" t="s">
+        <v>88</v>
+      </c>
+      <c r="E21" s="44" t="s">
+        <v>154</v>
+      </c>
+      <c r="F21" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="F21" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="G21" s="20" t="s">
+      <c r="G21" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="H21" s="20" t="s">
         <v>176</v>
       </c>
-      <c r="H21" s="31">
+      <c r="I21" s="31">
         <v>881.61</v>
       </c>
-      <c r="I21" s="21"/>
       <c r="J21" s="21"/>
-      <c r="K21" s="16">
-        <v>4800</v>
-      </c>
-      <c r="L21" s="21">
-        <v>3</v>
-      </c>
-      <c r="M21" s="38"/>
-      <c r="N21" s="17" t="s">
+      <c r="K21" s="21"/>
+      <c r="L21" s="16">
+        <v>4800</v>
+      </c>
+      <c r="M21" s="21">
+        <v>3</v>
+      </c>
+      <c r="N21" s="38"/>
+      <c r="O21" s="17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="20.100000000000001" customHeight="1">
+    <row r="22" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A22" s="3">
         <v>19</v>
       </c>
       <c r="B22" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="C22" s="55"/>
-      <c r="D22" s="46"/>
-      <c r="E22" s="18" t="s">
+      <c r="C22" s="49"/>
+      <c r="D22" s="60" t="s">
+        <v>88</v>
+      </c>
+      <c r="E22" s="44" t="s">
+        <v>154</v>
+      </c>
+      <c r="F22" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="F22" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="G22" s="20" t="s">
+      <c r="G22" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="H22" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="H22" s="33">
+      <c r="I22" s="33">
         <v>100.64</v>
       </c>
-      <c r="I22" s="21"/>
       <c r="J22" s="21"/>
-      <c r="K22" s="16">
-        <v>4800</v>
-      </c>
-      <c r="L22" s="21">
-        <v>3</v>
-      </c>
-      <c r="M22" s="38"/>
-      <c r="N22" s="17" t="s">
+      <c r="K22" s="21"/>
+      <c r="L22" s="16">
+        <v>4800</v>
+      </c>
+      <c r="M22" s="21">
+        <v>3</v>
+      </c>
+      <c r="N22" s="38"/>
+      <c r="O22" s="17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="20.100000000000001" customHeight="1">
+    <row r="23" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A23" s="3">
         <v>20</v>
       </c>
       <c r="B23" s="40" t="s">
         <v>107</v>
       </c>
-      <c r="C23" s="44" t="s">
+      <c r="C23" s="50" t="s">
         <v>148</v>
       </c>
-      <c r="D23" s="44" t="s">
+      <c r="D23" s="60" t="s">
         <v>147</v>
       </c>
-      <c r="E23" s="18" t="s">
+      <c r="E23" s="44" t="s">
+        <v>176</v>
+      </c>
+      <c r="F23" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="F23" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="G23" s="20" t="s">
+      <c r="G23" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="H23" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="H23" s="32">
+      <c r="I23" s="32">
         <v>99</v>
       </c>
-      <c r="I23" s="21"/>
       <c r="J23" s="21"/>
-      <c r="K23" s="16">
-        <v>4800</v>
-      </c>
-      <c r="L23" s="21">
-        <v>3</v>
-      </c>
-      <c r="M23" s="38"/>
-      <c r="N23" s="17" t="s">
+      <c r="K23" s="21"/>
+      <c r="L23" s="16">
+        <v>4800</v>
+      </c>
+      <c r="M23" s="21">
+        <v>3</v>
+      </c>
+      <c r="N23" s="38"/>
+      <c r="O23" s="17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="20.100000000000001" customHeight="1">
+    <row r="24" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A24" s="3">
         <v>21</v>
       </c>
       <c r="B24" s="41" t="s">
         <v>108</v>
       </c>
-      <c r="C24" s="45"/>
-      <c r="D24" s="45"/>
-      <c r="E24" s="18" t="s">
+      <c r="C24" s="52"/>
+      <c r="D24" s="60" t="s">
+        <v>147</v>
+      </c>
+      <c r="E24" s="44" t="s">
+        <v>176</v>
+      </c>
+      <c r="F24" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="F24" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="G24" s="20" t="s">
+      <c r="G24" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="H24" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="H24" s="27">
+      <c r="I24" s="27">
         <v>99</v>
       </c>
-      <c r="I24" s="21"/>
       <c r="J24" s="21"/>
-      <c r="K24" s="16">
-        <v>4800</v>
-      </c>
-      <c r="L24" s="21">
-        <v>3</v>
-      </c>
-      <c r="M24" s="38"/>
-      <c r="N24" s="17" t="s">
+      <c r="K24" s="21"/>
+      <c r="L24" s="16">
+        <v>4800</v>
+      </c>
+      <c r="M24" s="21">
+        <v>3</v>
+      </c>
+      <c r="N24" s="38"/>
+      <c r="O24" s="17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="20.100000000000001" customHeight="1">
+    <row r="25" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A25" s="3">
         <v>22</v>
       </c>
       <c r="B25" s="41" t="s">
         <v>109</v>
       </c>
-      <c r="C25" s="45"/>
-      <c r="D25" s="45"/>
-      <c r="E25" s="18" t="s">
+      <c r="C25" s="52"/>
+      <c r="D25" s="60" t="s">
+        <v>147</v>
+      </c>
+      <c r="E25" s="44" t="s">
+        <v>176</v>
+      </c>
+      <c r="F25" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="F25" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="G25" s="20" t="s">
+      <c r="G25" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="H25" s="20" t="s">
         <v>154</v>
       </c>
-      <c r="H25" s="27">
+      <c r="I25" s="27">
         <v>66</v>
       </c>
-      <c r="I25" s="21"/>
       <c r="J25" s="21"/>
-      <c r="K25" s="16">
-        <v>4800</v>
-      </c>
-      <c r="L25" s="21">
-        <v>3</v>
-      </c>
-      <c r="M25" s="38"/>
-      <c r="N25" s="17" t="s">
+      <c r="K25" s="21"/>
+      <c r="L25" s="16">
+        <v>4800</v>
+      </c>
+      <c r="M25" s="21">
+        <v>3</v>
+      </c>
+      <c r="N25" s="38"/>
+      <c r="O25" s="17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="20.100000000000001" customHeight="1">
+    <row r="26" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A26" s="3">
         <v>23</v>
       </c>
       <c r="B26" s="41" t="s">
         <v>110</v>
       </c>
-      <c r="C26" s="45"/>
-      <c r="D26" s="45"/>
-      <c r="E26" s="18" t="s">
+      <c r="C26" s="52"/>
+      <c r="D26" s="60" t="s">
+        <v>147</v>
+      </c>
+      <c r="E26" s="44" t="s">
+        <v>176</v>
+      </c>
+      <c r="F26" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="F26" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="G26" s="20" t="s">
+      <c r="G26" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="H26" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="H26" s="27">
+      <c r="I26" s="27">
         <v>66</v>
       </c>
-      <c r="I26" s="21"/>
       <c r="J26" s="21"/>
-      <c r="K26" s="16">
-        <v>4800</v>
-      </c>
-      <c r="L26" s="21">
-        <v>3</v>
-      </c>
-      <c r="M26" s="38"/>
-      <c r="N26" s="17" t="s">
+      <c r="K26" s="21"/>
+      <c r="L26" s="16">
+        <v>4800</v>
+      </c>
+      <c r="M26" s="21">
+        <v>3</v>
+      </c>
+      <c r="N26" s="38"/>
+      <c r="O26" s="17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="20.100000000000001" customHeight="1">
+    <row r="27" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A27" s="3">
         <v>24</v>
       </c>
       <c r="B27" s="41" t="s">
         <v>111</v>
       </c>
-      <c r="C27" s="45"/>
-      <c r="D27" s="45"/>
-      <c r="E27" s="18" t="s">
+      <c r="C27" s="52"/>
+      <c r="D27" s="60" t="s">
+        <v>147</v>
+      </c>
+      <c r="E27" s="44" t="s">
+        <v>176</v>
+      </c>
+      <c r="F27" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="F27" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="G27" s="20" t="s">
+      <c r="G27" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="H27" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="H27" s="27">
+      <c r="I27" s="27">
         <v>415.87</v>
       </c>
-      <c r="I27" s="21"/>
       <c r="J27" s="21"/>
-      <c r="K27" s="16">
-        <v>4800</v>
-      </c>
-      <c r="L27" s="21">
-        <v>3</v>
-      </c>
-      <c r="M27" s="38"/>
-      <c r="N27" s="17" t="s">
+      <c r="K27" s="21"/>
+      <c r="L27" s="16">
+        <v>4800</v>
+      </c>
+      <c r="M27" s="21">
+        <v>3</v>
+      </c>
+      <c r="N27" s="38"/>
+      <c r="O27" s="17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="20.100000000000001" customHeight="1">
+    <row r="28" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A28" s="3">
         <v>25</v>
       </c>
       <c r="B28" s="41" t="s">
         <v>112</v>
       </c>
-      <c r="C28" s="45"/>
-      <c r="D28" s="45"/>
-      <c r="E28" s="18" t="s">
+      <c r="C28" s="52"/>
+      <c r="D28" s="60" t="s">
+        <v>147</v>
+      </c>
+      <c r="E28" s="44" t="s">
+        <v>176</v>
+      </c>
+      <c r="F28" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="F28" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="G28" s="20" t="s">
+      <c r="G28" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="H28" s="20" t="s">
         <v>176</v>
       </c>
-      <c r="H28" s="27">
+      <c r="I28" s="27">
         <v>456.72</v>
       </c>
-      <c r="I28" s="21"/>
       <c r="J28" s="21"/>
-      <c r="K28" s="16">
-        <v>4800</v>
-      </c>
-      <c r="L28" s="21">
-        <v>3</v>
-      </c>
-      <c r="M28" s="38"/>
-      <c r="N28" s="17" t="s">
+      <c r="K28" s="21"/>
+      <c r="L28" s="16">
+        <v>4800</v>
+      </c>
+      <c r="M28" s="21">
+        <v>3</v>
+      </c>
+      <c r="N28" s="38"/>
+      <c r="O28" s="17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="20.100000000000001" customHeight="1">
+    <row r="29" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A29" s="3">
         <v>26</v>
       </c>
       <c r="B29" s="41" t="s">
         <v>113</v>
       </c>
-      <c r="C29" s="45"/>
-      <c r="D29" s="45"/>
-      <c r="E29" s="18" t="s">
+      <c r="C29" s="52"/>
+      <c r="D29" s="60" t="s">
+        <v>147</v>
+      </c>
+      <c r="E29" s="44" t="s">
+        <v>176</v>
+      </c>
+      <c r="F29" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="F29" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="G29" s="20" t="s">
+      <c r="G29" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="H29" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="H29" s="27">
+      <c r="I29" s="27">
         <v>265.76</v>
       </c>
-      <c r="I29" s="21"/>
       <c r="J29" s="21"/>
-      <c r="K29" s="16">
-        <v>4800</v>
-      </c>
-      <c r="L29" s="21">
-        <v>3</v>
-      </c>
-      <c r="M29" s="38"/>
-      <c r="N29" s="17" t="s">
+      <c r="K29" s="21"/>
+      <c r="L29" s="16">
+        <v>4800</v>
+      </c>
+      <c r="M29" s="21">
+        <v>3</v>
+      </c>
+      <c r="N29" s="38"/>
+      <c r="O29" s="17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="20.100000000000001" customHeight="1">
+    <row r="30" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A30" s="3">
         <v>27</v>
       </c>
       <c r="B30" s="41" t="s">
         <v>114</v>
       </c>
-      <c r="C30" s="45"/>
-      <c r="D30" s="45"/>
-      <c r="E30" s="18" t="s">
+      <c r="C30" s="52"/>
+      <c r="D30" s="60" t="s">
+        <v>147</v>
+      </c>
+      <c r="E30" s="44" t="s">
+        <v>176</v>
+      </c>
+      <c r="F30" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="F30" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="G30" s="20" t="s">
+      <c r="G30" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="H30" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="H30" s="27">
+      <c r="I30" s="27">
         <v>111.3</v>
       </c>
-      <c r="I30" s="21"/>
       <c r="J30" s="21"/>
-      <c r="K30" s="16">
-        <v>4800</v>
-      </c>
-      <c r="L30" s="21">
-        <v>3</v>
-      </c>
-      <c r="M30" s="38"/>
-      <c r="N30" s="17" t="s">
+      <c r="K30" s="21"/>
+      <c r="L30" s="16">
+        <v>4800</v>
+      </c>
+      <c r="M30" s="21">
+        <v>3</v>
+      </c>
+      <c r="N30" s="38"/>
+      <c r="O30" s="17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="20.100000000000001" customHeight="1">
+    <row r="31" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A31" s="3">
         <v>28</v>
       </c>
       <c r="B31" s="41" t="s">
         <v>115</v>
       </c>
-      <c r="C31" s="45"/>
-      <c r="D31" s="46"/>
-      <c r="E31" s="18" t="s">
+      <c r="C31" s="52"/>
+      <c r="D31" s="60" t="s">
+        <v>147</v>
+      </c>
+      <c r="E31" s="44" t="s">
+        <v>176</v>
+      </c>
+      <c r="F31" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="F31" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="G31" s="20" t="s">
+      <c r="G31" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="H31" s="20" t="s">
         <v>176</v>
       </c>
-      <c r="H31" s="27">
+      <c r="I31" s="27">
         <v>859.76</v>
       </c>
-      <c r="I31" s="21"/>
       <c r="J31" s="21"/>
-      <c r="K31" s="16">
-        <v>4800</v>
-      </c>
-      <c r="L31" s="21">
-        <v>3</v>
-      </c>
-      <c r="M31" s="38"/>
-      <c r="N31" s="17" t="s">
+      <c r="K31" s="21"/>
+      <c r="L31" s="16">
+        <v>4800</v>
+      </c>
+      <c r="M31" s="21">
+        <v>3</v>
+      </c>
+      <c r="N31" s="38"/>
+      <c r="O31" s="17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="20.100000000000001" customHeight="1">
+    <row r="32" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A32" s="3">
         <v>29</v>
       </c>
       <c r="B32" s="42" t="s">
         <v>116</v>
       </c>
-      <c r="C32" s="45"/>
-      <c r="D32" s="44" t="s">
+      <c r="C32" s="52"/>
+      <c r="D32" s="60" t="s">
         <v>89</v>
       </c>
-      <c r="E32" s="18" t="s">
+      <c r="E32" s="44" t="s">
+        <v>176</v>
+      </c>
+      <c r="F32" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="F32" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="G32" s="20" t="s">
+      <c r="G32" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="H32" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="H32" s="27">
+      <c r="I32" s="27">
         <v>202.92</v>
       </c>
-      <c r="I32" s="21"/>
       <c r="J32" s="21"/>
-      <c r="K32" s="16">
-        <v>4800</v>
-      </c>
-      <c r="L32" s="21">
-        <v>3</v>
-      </c>
-      <c r="M32" s="38"/>
-      <c r="N32" s="17" t="s">
+      <c r="K32" s="21"/>
+      <c r="L32" s="16">
+        <v>4800</v>
+      </c>
+      <c r="M32" s="21">
+        <v>3</v>
+      </c>
+      <c r="N32" s="38"/>
+      <c r="O32" s="17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="20.100000000000001" customHeight="1">
+    <row r="33" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A33" s="3">
         <v>30</v>
       </c>
       <c r="B33" s="41" t="s">
         <v>117</v>
       </c>
-      <c r="C33" s="45"/>
-      <c r="D33" s="45"/>
-      <c r="E33" s="18" t="s">
+      <c r="C33" s="52"/>
+      <c r="D33" s="60" t="s">
+        <v>89</v>
+      </c>
+      <c r="E33" s="44" t="s">
+        <v>1</v>
+      </c>
+      <c r="F33" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="F33" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="G33" s="20" t="s">
+      <c r="G33" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="H33" s="20" t="s">
         <v>174</v>
       </c>
-      <c r="H33" s="27">
+      <c r="I33" s="27">
         <v>132</v>
       </c>
-      <c r="I33" s="21"/>
       <c r="J33" s="21"/>
-      <c r="K33" s="16">
-        <v>4800</v>
-      </c>
-      <c r="L33" s="21">
-        <v>3</v>
-      </c>
-      <c r="M33" s="38"/>
-      <c r="N33" s="17" t="s">
+      <c r="K33" s="21"/>
+      <c r="L33" s="16">
+        <v>4800</v>
+      </c>
+      <c r="M33" s="21">
+        <v>3</v>
+      </c>
+      <c r="N33" s="38"/>
+      <c r="O33" s="17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="20.100000000000001" customHeight="1">
+    <row r="34" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A34" s="3">
         <v>31</v>
       </c>
       <c r="B34" s="41" t="s">
         <v>118</v>
       </c>
-      <c r="C34" s="45"/>
-      <c r="D34" s="45"/>
-      <c r="E34" s="18" t="s">
+      <c r="C34" s="52"/>
+      <c r="D34" s="60" t="s">
+        <v>89</v>
+      </c>
+      <c r="E34" s="44" t="s">
+        <v>1</v>
+      </c>
+      <c r="F34" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="F34" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="G34" s="20" t="s">
+      <c r="G34" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="H34" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="H34" s="27">
+      <c r="I34" s="27">
         <v>118.8</v>
       </c>
-      <c r="I34" s="21"/>
       <c r="J34" s="21"/>
-      <c r="K34" s="16">
-        <v>4800</v>
-      </c>
-      <c r="L34" s="21">
-        <v>3</v>
-      </c>
-      <c r="M34" s="38"/>
-      <c r="N34" s="17" t="s">
+      <c r="K34" s="21"/>
+      <c r="L34" s="16">
+        <v>4800</v>
+      </c>
+      <c r="M34" s="21">
+        <v>3</v>
+      </c>
+      <c r="N34" s="38"/>
+      <c r="O34" s="17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="20.100000000000001" customHeight="1">
+    <row r="35" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A35" s="3">
         <v>32</v>
       </c>
       <c r="B35" s="41" t="s">
         <v>119</v>
       </c>
-      <c r="C35" s="45"/>
-      <c r="D35" s="45"/>
-      <c r="E35" s="18" t="s">
+      <c r="C35" s="52"/>
+      <c r="D35" s="60" t="s">
+        <v>89</v>
+      </c>
+      <c r="E35" s="44" t="s">
+        <v>1</v>
+      </c>
+      <c r="F35" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="F35" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="G35" s="20" t="s">
+      <c r="G35" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="H35" s="20" t="s">
         <v>175</v>
       </c>
-      <c r="H35" s="28">
+      <c r="I35" s="28">
         <v>1083.68</v>
       </c>
-      <c r="I35" s="21"/>
       <c r="J35" s="21"/>
-      <c r="K35" s="16">
-        <v>4800</v>
-      </c>
-      <c r="L35" s="21">
-        <v>3</v>
-      </c>
-      <c r="M35" s="38"/>
-      <c r="N35" s="17" t="s">
+      <c r="K35" s="21"/>
+      <c r="L35" s="16">
+        <v>4800</v>
+      </c>
+      <c r="M35" s="21">
+        <v>3</v>
+      </c>
+      <c r="N35" s="38"/>
+      <c r="O35" s="17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="20.100000000000001" customHeight="1">
+    <row r="36" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A36" s="3">
         <v>33</v>
       </c>
       <c r="B36" s="41" t="s">
         <v>120</v>
       </c>
-      <c r="C36" s="45"/>
-      <c r="D36" s="45"/>
-      <c r="E36" s="18" t="s">
+      <c r="C36" s="52"/>
+      <c r="D36" s="60" t="s">
+        <v>89</v>
+      </c>
+      <c r="E36" s="44" t="s">
+        <v>1</v>
+      </c>
+      <c r="F36" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="F36" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="G36" s="20" t="s">
+      <c r="G36" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="H36" s="20" t="s">
         <v>174</v>
       </c>
-      <c r="H36" s="27">
+      <c r="I36" s="27">
         <v>334.88</v>
       </c>
-      <c r="I36" s="21"/>
       <c r="J36" s="21"/>
-      <c r="K36" s="16">
-        <v>4800</v>
-      </c>
-      <c r="L36" s="21">
-        <v>3</v>
-      </c>
-      <c r="M36" s="38"/>
-      <c r="N36" s="17" t="s">
+      <c r="K36" s="21"/>
+      <c r="L36" s="16">
+        <v>4800</v>
+      </c>
+      <c r="M36" s="21">
+        <v>3</v>
+      </c>
+      <c r="N36" s="38"/>
+      <c r="O36" s="17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="20.100000000000001" customHeight="1">
+    <row r="37" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A37" s="3">
         <v>34</v>
       </c>
       <c r="B37" s="41" t="s">
         <v>121</v>
       </c>
-      <c r="C37" s="45"/>
-      <c r="D37" s="44" t="s">
+      <c r="C37" s="52"/>
+      <c r="D37" s="60" t="s">
         <v>88</v>
       </c>
-      <c r="E37" s="18" t="s">
+      <c r="E37" s="44" t="s">
+        <v>1</v>
+      </c>
+      <c r="F37" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="F37" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="G37" s="20" t="s">
+      <c r="G37" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="H37" s="20" t="s">
         <v>176</v>
       </c>
-      <c r="H37" s="27">
+      <c r="I37" s="27">
         <v>931.35</v>
       </c>
-      <c r="I37" s="21"/>
       <c r="J37" s="21"/>
-      <c r="K37" s="16">
-        <v>4800</v>
-      </c>
-      <c r="L37" s="21">
-        <v>3</v>
-      </c>
-      <c r="M37" s="38"/>
-      <c r="N37" s="17" t="s">
+      <c r="K37" s="21"/>
+      <c r="L37" s="16">
+        <v>4800</v>
+      </c>
+      <c r="M37" s="21">
+        <v>3</v>
+      </c>
+      <c r="N37" s="38"/>
+      <c r="O37" s="17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="20.100000000000001" customHeight="1">
+    <row r="38" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A38" s="3">
         <v>35</v>
       </c>
       <c r="B38" s="41" t="s">
         <v>122</v>
       </c>
-      <c r="C38" s="45"/>
-      <c r="D38" s="45"/>
-      <c r="E38" s="18" t="s">
+      <c r="C38" s="52"/>
+      <c r="D38" s="60" t="s">
+        <v>88</v>
+      </c>
+      <c r="E38" s="45" t="s">
+        <v>174</v>
+      </c>
+      <c r="F38" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="F38" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="G38" s="20" t="s">
+      <c r="G38" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="H38" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="H38" s="27">
+      <c r="I38" s="27">
         <v>329.88</v>
       </c>
-      <c r="I38" s="21"/>
       <c r="J38" s="21"/>
-      <c r="K38" s="16">
-        <v>4800</v>
-      </c>
-      <c r="L38" s="21">
-        <v>3</v>
-      </c>
-      <c r="M38" s="38"/>
-      <c r="N38" s="17" t="s">
+      <c r="K38" s="21"/>
+      <c r="L38" s="16">
+        <v>4800</v>
+      </c>
+      <c r="M38" s="21">
+        <v>3</v>
+      </c>
+      <c r="N38" s="38"/>
+      <c r="O38" s="17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="39" spans="1:14" ht="20.100000000000001" customHeight="1">
+    <row r="39" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A39" s="3">
         <v>36</v>
       </c>
       <c r="B39" s="41" t="s">
         <v>123</v>
       </c>
-      <c r="C39" s="45"/>
-      <c r="D39" s="45"/>
-      <c r="E39" s="18" t="s">
+      <c r="C39" s="52"/>
+      <c r="D39" s="60" t="s">
+        <v>88</v>
+      </c>
+      <c r="E39" s="45" t="s">
+        <v>174</v>
+      </c>
+      <c r="F39" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="F39" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="G39" s="20" t="s">
+      <c r="G39" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="H39" s="20" t="s">
         <v>173</v>
       </c>
-      <c r="H39" s="27">
+      <c r="I39" s="27">
         <v>282.39999999999998</v>
       </c>
-      <c r="I39" s="21"/>
       <c r="J39" s="21"/>
-      <c r="K39" s="16">
-        <v>4800</v>
-      </c>
-      <c r="L39" s="21">
-        <v>3</v>
-      </c>
-      <c r="M39" s="38"/>
-      <c r="N39" s="17" t="s">
+      <c r="K39" s="21"/>
+      <c r="L39" s="16">
+        <v>4800</v>
+      </c>
+      <c r="M39" s="21">
+        <v>3</v>
+      </c>
+      <c r="N39" s="38"/>
+      <c r="O39" s="17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="40" spans="1:14" ht="20.100000000000001" customHeight="1">
+    <row r="40" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A40" s="3">
         <v>37</v>
       </c>
       <c r="B40" s="41" t="s">
         <v>124</v>
       </c>
-      <c r="C40" s="45"/>
-      <c r="D40" s="45"/>
-      <c r="E40" s="18" t="s">
+      <c r="C40" s="52"/>
+      <c r="D40" s="60" t="s">
+        <v>88</v>
+      </c>
+      <c r="E40" s="45" t="s">
+        <v>174</v>
+      </c>
+      <c r="F40" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="F40" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="G40" s="20" t="s">
+      <c r="G40" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="H40" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="H40" s="27">
+      <c r="I40" s="27">
         <v>64.8</v>
       </c>
-      <c r="I40" s="21"/>
       <c r="J40" s="21"/>
-      <c r="K40" s="16">
-        <v>4800</v>
-      </c>
-      <c r="L40" s="21">
-        <v>3</v>
-      </c>
-      <c r="M40" s="38"/>
-      <c r="N40" s="17" t="s">
+      <c r="K40" s="21"/>
+      <c r="L40" s="16">
+        <v>4800</v>
+      </c>
+      <c r="M40" s="21">
+        <v>3</v>
+      </c>
+      <c r="N40" s="38"/>
+      <c r="O40" s="17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="1:14" ht="20.100000000000001" customHeight="1">
+    <row r="41" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A41" s="3">
         <v>38</v>
       </c>
       <c r="B41" s="41" t="s">
         <v>125</v>
       </c>
-      <c r="C41" s="45"/>
-      <c r="D41" s="45"/>
-      <c r="E41" s="18" t="s">
+      <c r="C41" s="52"/>
+      <c r="D41" s="60" t="s">
+        <v>88</v>
+      </c>
+      <c r="E41" s="45" t="s">
+        <v>174</v>
+      </c>
+      <c r="F41" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="F41" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="G41" s="20" t="s">
+      <c r="G41" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="H41" s="20" t="s">
         <v>177</v>
       </c>
-      <c r="H41" s="27">
+      <c r="I41" s="27">
         <v>135.88</v>
       </c>
-      <c r="I41" s="21"/>
       <c r="J41" s="21"/>
-      <c r="K41" s="16">
-        <v>4800</v>
-      </c>
-      <c r="L41" s="21">
-        <v>3</v>
-      </c>
-      <c r="M41" s="38"/>
-      <c r="N41" s="17" t="s">
+      <c r="K41" s="21"/>
+      <c r="L41" s="16">
+        <v>4800</v>
+      </c>
+      <c r="M41" s="21">
+        <v>3</v>
+      </c>
+      <c r="N41" s="38"/>
+      <c r="O41" s="17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="42" spans="1:14" ht="20.100000000000001" customHeight="1">
+    <row r="42" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A42" s="3">
         <v>39</v>
       </c>
       <c r="B42" s="41" t="s">
         <v>82</v>
       </c>
-      <c r="C42" s="45"/>
-      <c r="D42" s="45"/>
-      <c r="E42" s="18" t="s">
+      <c r="C42" s="52"/>
+      <c r="D42" s="60" t="s">
+        <v>88</v>
+      </c>
+      <c r="E42" s="45" t="s">
+        <v>174</v>
+      </c>
+      <c r="F42" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="F42" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="G42" s="20" t="s">
+      <c r="G42" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="H42" s="20" t="s">
         <v>176</v>
       </c>
-      <c r="H42" s="27">
+      <c r="I42" s="27">
         <v>64.8</v>
       </c>
-      <c r="I42" s="21"/>
       <c r="J42" s="21"/>
-      <c r="K42" s="16">
-        <v>4800</v>
-      </c>
-      <c r="L42" s="21">
-        <v>3</v>
-      </c>
-      <c r="M42" s="38"/>
-      <c r="N42" s="17" t="s">
+      <c r="K42" s="21"/>
+      <c r="L42" s="16">
+        <v>4800</v>
+      </c>
+      <c r="M42" s="21">
+        <v>3</v>
+      </c>
+      <c r="N42" s="38"/>
+      <c r="O42" s="17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="43" spans="1:14" ht="20.100000000000001" customHeight="1">
+    <row r="43" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A43" s="3">
         <v>40</v>
       </c>
       <c r="B43" s="41" t="s">
         <v>126</v>
       </c>
-      <c r="C43" s="45"/>
-      <c r="D43" s="45"/>
-      <c r="E43" s="18" t="s">
+      <c r="C43" s="52"/>
+      <c r="D43" s="60" t="s">
+        <v>88</v>
+      </c>
+      <c r="E43" s="45" t="s">
+        <v>174</v>
+      </c>
+      <c r="F43" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="F43" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="G43" s="20" t="s">
+      <c r="G43" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="H43" s="20" t="s">
         <v>174</v>
       </c>
-      <c r="H43" s="27">
+      <c r="I43" s="27">
         <v>609.76</v>
       </c>
-      <c r="I43" s="21"/>
       <c r="J43" s="21"/>
-      <c r="K43" s="16">
-        <v>4800</v>
-      </c>
-      <c r="L43" s="21">
-        <v>3</v>
-      </c>
-      <c r="M43" s="38"/>
-      <c r="N43" s="17" t="s">
+      <c r="K43" s="21"/>
+      <c r="L43" s="16">
+        <v>4800</v>
+      </c>
+      <c r="M43" s="21">
+        <v>3</v>
+      </c>
+      <c r="N43" s="38"/>
+      <c r="O43" s="17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="44" spans="1:14" ht="20.100000000000001" customHeight="1">
+    <row r="44" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A44" s="3">
         <v>41</v>
       </c>
       <c r="B44" s="41" t="s">
         <v>127</v>
       </c>
-      <c r="C44" s="45"/>
-      <c r="D44" s="45"/>
-      <c r="E44" s="18" t="s">
+      <c r="C44" s="52"/>
+      <c r="D44" s="60" t="s">
+        <v>88</v>
+      </c>
+      <c r="E44" s="45" t="s">
+        <v>174</v>
+      </c>
+      <c r="F44" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="F44" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="G44" s="20" t="s">
+      <c r="G44" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="H44" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="H44" s="27">
+      <c r="I44" s="27">
         <v>602.96</v>
       </c>
-      <c r="I44" s="21"/>
       <c r="J44" s="21"/>
-      <c r="K44" s="16">
-        <v>4800</v>
-      </c>
-      <c r="L44" s="21">
-        <v>3</v>
-      </c>
-      <c r="M44" s="38"/>
-      <c r="N44" s="17" t="s">
+      <c r="K44" s="21"/>
+      <c r="L44" s="16">
+        <v>4800</v>
+      </c>
+      <c r="M44" s="21">
+        <v>3</v>
+      </c>
+      <c r="N44" s="38"/>
+      <c r="O44" s="17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="45" spans="1:14" ht="20.100000000000001" customHeight="1">
+    <row r="45" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A45" s="3">
         <v>42</v>
       </c>
       <c r="B45" s="41" t="s">
         <v>128</v>
       </c>
-      <c r="C45" s="45"/>
-      <c r="D45" s="45"/>
-      <c r="E45" s="18" t="s">
+      <c r="C45" s="52"/>
+      <c r="D45" s="60" t="s">
+        <v>88</v>
+      </c>
+      <c r="E45" s="45" t="s">
+        <v>174</v>
+      </c>
+      <c r="F45" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="F45" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="G45" s="20" t="s">
+      <c r="G45" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="H45" s="20" t="s">
         <v>153</v>
       </c>
-      <c r="H45" s="27">
+      <c r="I45" s="27">
         <v>59.84</v>
       </c>
-      <c r="I45" s="21"/>
       <c r="J45" s="21"/>
-      <c r="K45" s="16">
-        <v>4800</v>
-      </c>
-      <c r="L45" s="21">
-        <v>3</v>
-      </c>
-      <c r="M45" s="38"/>
-      <c r="N45" s="17" t="s">
+      <c r="K45" s="21"/>
+      <c r="L45" s="16">
+        <v>4800</v>
+      </c>
+      <c r="M45" s="21">
+        <v>3</v>
+      </c>
+      <c r="N45" s="38"/>
+      <c r="O45" s="17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="46" spans="1:14" ht="20.100000000000001" customHeight="1">
+    <row r="46" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A46" s="3">
         <v>43</v>
       </c>
       <c r="B46" s="41" t="s">
         <v>129</v>
       </c>
-      <c r="C46" s="45"/>
-      <c r="D46" s="45"/>
-      <c r="E46" s="18" t="s">
+      <c r="C46" s="52"/>
+      <c r="D46" s="60" t="s">
+        <v>88</v>
+      </c>
+      <c r="E46" s="45" t="s">
+        <v>174</v>
+      </c>
+      <c r="F46" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="F46" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="G46" s="20" t="s">
+      <c r="G46" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="H46" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="H46" s="27">
+      <c r="I46" s="27">
         <v>90.8</v>
       </c>
-      <c r="I46" s="21"/>
       <c r="J46" s="21"/>
-      <c r="K46" s="16">
-        <v>4800</v>
-      </c>
-      <c r="L46" s="21">
-        <v>3</v>
-      </c>
-      <c r="M46" s="38"/>
-      <c r="N46" s="17" t="s">
+      <c r="K46" s="21"/>
+      <c r="L46" s="16">
+        <v>4800</v>
+      </c>
+      <c r="M46" s="21">
+        <v>3</v>
+      </c>
+      <c r="N46" s="38"/>
+      <c r="O46" s="17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="47" spans="1:14" ht="20.100000000000001" customHeight="1">
+    <row r="47" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A47" s="3">
         <v>44</v>
       </c>
       <c r="B47" s="41" t="s">
         <v>130</v>
       </c>
-      <c r="C47" s="45"/>
-      <c r="D47" s="45"/>
-      <c r="E47" s="18" t="s">
+      <c r="C47" s="52"/>
+      <c r="D47" s="60" t="s">
+        <v>88</v>
+      </c>
+      <c r="E47" s="45" t="s">
+        <v>174</v>
+      </c>
+      <c r="F47" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="F47" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="G47" s="20" t="s">
+      <c r="G47" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="H47" s="20" t="s">
         <v>178</v>
       </c>
-      <c r="H47" s="27">
+      <c r="I47" s="27">
         <v>318.56</v>
       </c>
-      <c r="I47" s="21"/>
       <c r="J47" s="21"/>
-      <c r="K47" s="16">
-        <v>4800</v>
-      </c>
-      <c r="L47" s="21">
-        <v>3</v>
-      </c>
-      <c r="M47" s="38"/>
-      <c r="N47" s="17" t="s">
+      <c r="K47" s="21"/>
+      <c r="L47" s="16">
+        <v>4800</v>
+      </c>
+      <c r="M47" s="21">
+        <v>3</v>
+      </c>
+      <c r="N47" s="38"/>
+      <c r="O47" s="17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="48" spans="1:14" ht="20.100000000000001" customHeight="1">
+    <row r="48" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A48" s="3">
         <v>45</v>
       </c>
       <c r="B48" s="41" t="s">
         <v>131</v>
       </c>
-      <c r="C48" s="45"/>
-      <c r="D48" s="45"/>
-      <c r="E48" s="18" t="s">
+      <c r="C48" s="52"/>
+      <c r="D48" s="60" t="s">
+        <v>88</v>
+      </c>
+      <c r="E48" s="45" t="s">
+        <v>174</v>
+      </c>
+      <c r="F48" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="F48" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="G48" s="20" t="s">
+      <c r="G48" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="H48" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="H48" s="27">
+      <c r="I48" s="27">
         <v>63</v>
       </c>
-      <c r="I48" s="21"/>
       <c r="J48" s="21"/>
-      <c r="K48" s="16">
-        <v>4800</v>
-      </c>
-      <c r="L48" s="21">
-        <v>3</v>
-      </c>
-      <c r="M48" s="38"/>
-      <c r="N48" s="17" t="s">
+      <c r="K48" s="21"/>
+      <c r="L48" s="16">
+        <v>4800</v>
+      </c>
+      <c r="M48" s="21">
+        <v>3</v>
+      </c>
+      <c r="N48" s="38"/>
+      <c r="O48" s="17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="49" spans="1:14" ht="20.100000000000001" customHeight="1">
+    <row r="49" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A49" s="3">
         <v>46</v>
       </c>
       <c r="B49" s="41" t="s">
         <v>84</v>
       </c>
-      <c r="C49" s="45"/>
-      <c r="D49" s="45"/>
-      <c r="E49" s="18" t="s">
+      <c r="C49" s="52"/>
+      <c r="D49" s="60" t="s">
+        <v>88</v>
+      </c>
+      <c r="E49" s="45" t="s">
+        <v>174</v>
+      </c>
+      <c r="F49" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="F49" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="G49" s="20" t="s">
+      <c r="G49" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="H49" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="H49" s="27">
+      <c r="I49" s="27">
         <v>464.56</v>
       </c>
-      <c r="I49" s="21"/>
       <c r="J49" s="21"/>
-      <c r="K49" s="16">
-        <v>4800</v>
-      </c>
-      <c r="L49" s="21">
-        <v>3</v>
-      </c>
-      <c r="M49" s="38"/>
-      <c r="N49" s="17" t="s">
+      <c r="K49" s="21"/>
+      <c r="L49" s="16">
+        <v>4800</v>
+      </c>
+      <c r="M49" s="21">
+        <v>3</v>
+      </c>
+      <c r="N49" s="38"/>
+      <c r="O49" s="17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="50" spans="1:14" ht="20.100000000000001" customHeight="1">
+    <row r="50" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A50" s="3">
         <v>47</v>
       </c>
       <c r="B50" s="41" t="s">
         <v>85</v>
       </c>
-      <c r="C50" s="45"/>
-      <c r="D50" s="45"/>
-      <c r="E50" s="18" t="s">
+      <c r="C50" s="52"/>
+      <c r="D50" s="60" t="s">
+        <v>88</v>
+      </c>
+      <c r="E50" s="45" t="s">
+        <v>174</v>
+      </c>
+      <c r="F50" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="F50" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="G50" s="20" t="s">
+      <c r="G50" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="H50" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="H50" s="27">
+      <c r="I50" s="27">
         <v>126.36</v>
       </c>
-      <c r="I50" s="21"/>
       <c r="J50" s="21"/>
-      <c r="K50" s="16">
-        <v>4800</v>
-      </c>
-      <c r="L50" s="21">
-        <v>3</v>
-      </c>
-      <c r="M50" s="38"/>
-      <c r="N50" s="17" t="s">
+      <c r="K50" s="21"/>
+      <c r="L50" s="16">
+        <v>4800</v>
+      </c>
+      <c r="M50" s="21">
+        <v>3</v>
+      </c>
+      <c r="N50" s="38"/>
+      <c r="O50" s="17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="51" spans="1:14" ht="20.100000000000001" customHeight="1">
+    <row r="51" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A51" s="3">
         <v>48</v>
       </c>
       <c r="B51" s="41" t="s">
         <v>132</v>
       </c>
-      <c r="C51" s="45"/>
-      <c r="D51" s="45"/>
-      <c r="E51" s="18" t="s">
+      <c r="C51" s="52"/>
+      <c r="D51" s="60" t="s">
+        <v>88</v>
+      </c>
+      <c r="E51" s="45" t="s">
+        <v>174</v>
+      </c>
+      <c r="F51" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="F51" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="G51" s="20" t="s">
+      <c r="G51" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="H51" s="20" t="s">
         <v>174</v>
       </c>
-      <c r="H51" s="27">
+      <c r="I51" s="27">
         <v>148.52000000000001</v>
       </c>
-      <c r="I51" s="21"/>
       <c r="J51" s="21"/>
-      <c r="K51" s="16">
-        <v>4800</v>
-      </c>
-      <c r="L51" s="21">
-        <v>3</v>
-      </c>
-      <c r="M51" s="38"/>
-      <c r="N51" s="17" t="s">
+      <c r="K51" s="21"/>
+      <c r="L51" s="16">
+        <v>4800</v>
+      </c>
+      <c r="M51" s="21">
+        <v>3</v>
+      </c>
+      <c r="N51" s="38"/>
+      <c r="O51" s="17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="52" spans="1:14" ht="20.100000000000001" customHeight="1">
+    <row r="52" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A52" s="3">
         <v>49</v>
       </c>
       <c r="B52" s="41" t="s">
         <v>133</v>
       </c>
-      <c r="C52" s="45"/>
-      <c r="D52" s="45"/>
-      <c r="E52" s="18" t="s">
+      <c r="C52" s="52"/>
+      <c r="D52" s="60" t="s">
+        <v>88</v>
+      </c>
+      <c r="E52" s="45" t="s">
+        <v>174</v>
+      </c>
+      <c r="F52" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="F52" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="G52" s="20" t="s">
+      <c r="G52" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="H52" s="20" t="s">
         <v>177</v>
       </c>
-      <c r="H52" s="27">
+      <c r="I52" s="27">
         <v>511.44</v>
       </c>
-      <c r="I52" s="21"/>
       <c r="J52" s="21"/>
-      <c r="K52" s="16">
-        <v>4800</v>
-      </c>
-      <c r="L52" s="21">
-        <v>3</v>
-      </c>
-      <c r="M52" s="38"/>
-      <c r="N52" s="17" t="s">
+      <c r="K52" s="21"/>
+      <c r="L52" s="16">
+        <v>4800</v>
+      </c>
+      <c r="M52" s="21">
+        <v>3</v>
+      </c>
+      <c r="N52" s="38"/>
+      <c r="O52" s="17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="53" spans="1:14" ht="20.100000000000001" customHeight="1">
+    <row r="53" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A53" s="3">
         <v>50</v>
       </c>
       <c r="B53" s="41" t="s">
         <v>134</v>
       </c>
-      <c r="C53" s="45"/>
-      <c r="D53" s="45"/>
-      <c r="E53" s="18" t="s">
+      <c r="C53" s="52"/>
+      <c r="D53" s="60" t="s">
+        <v>88</v>
+      </c>
+      <c r="E53" s="45" t="s">
+        <v>174</v>
+      </c>
+      <c r="F53" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="F53" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="G53" s="20" t="s">
+      <c r="G53" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="H53" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="H53" s="27">
+      <c r="I53" s="27">
         <v>31.5</v>
       </c>
-      <c r="I53" s="21"/>
       <c r="J53" s="21"/>
-      <c r="K53" s="16">
-        <v>4800</v>
-      </c>
-      <c r="L53" s="21">
-        <v>3</v>
-      </c>
-      <c r="M53" s="38"/>
-      <c r="N53" s="17" t="s">
+      <c r="K53" s="21"/>
+      <c r="L53" s="16">
+        <v>4800</v>
+      </c>
+      <c r="M53" s="21">
+        <v>3</v>
+      </c>
+      <c r="N53" s="38"/>
+      <c r="O53" s="17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="54" spans="1:14" ht="20.100000000000001" customHeight="1">
+    <row r="54" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A54" s="3">
         <v>51</v>
       </c>
       <c r="B54" s="41" t="s">
         <v>79</v>
       </c>
-      <c r="C54" s="45"/>
-      <c r="D54" s="45"/>
-      <c r="E54" s="18" t="s">
+      <c r="C54" s="52"/>
+      <c r="D54" s="60" t="s">
+        <v>88</v>
+      </c>
+      <c r="E54" s="45" t="s">
+        <v>174</v>
+      </c>
+      <c r="F54" s="18" t="s">
         <v>140</v>
       </c>
-      <c r="F54" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="G54" s="20" t="s">
+      <c r="G54" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="H54" s="20" t="s">
         <v>176</v>
       </c>
-      <c r="H54" s="27">
+      <c r="I54" s="27">
         <v>60.96</v>
       </c>
-      <c r="I54" s="21"/>
       <c r="J54" s="21"/>
-      <c r="K54" s="16">
-        <v>4800</v>
-      </c>
-      <c r="L54" s="21">
-        <v>3</v>
-      </c>
-      <c r="M54" s="38"/>
-      <c r="N54" s="17" t="s">
+      <c r="K54" s="21"/>
+      <c r="L54" s="16">
+        <v>4800</v>
+      </c>
+      <c r="M54" s="21">
+        <v>3</v>
+      </c>
+      <c r="N54" s="38"/>
+      <c r="O54" s="17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="55" spans="1:14" ht="20.100000000000001" customHeight="1">
+    <row r="55" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A55" s="3">
         <v>52</v>
       </c>
       <c r="B55" s="41" t="s">
         <v>135</v>
       </c>
-      <c r="C55" s="45"/>
-      <c r="D55" s="45"/>
-      <c r="E55" s="18" t="s">
+      <c r="C55" s="52"/>
+      <c r="D55" s="60" t="s">
+        <v>88</v>
+      </c>
+      <c r="E55" s="45" t="s">
+        <v>174</v>
+      </c>
+      <c r="F55" s="18" t="s">
         <v>141</v>
       </c>
-      <c r="F55" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="G55" s="20" t="s">
+      <c r="G55" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="H55" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="H55" s="27">
+      <c r="I55" s="27">
         <v>826.56</v>
       </c>
-      <c r="I55" s="21"/>
       <c r="J55" s="21"/>
-      <c r="K55" s="16">
-        <v>4800</v>
-      </c>
-      <c r="L55" s="21">
-        <v>3</v>
-      </c>
-      <c r="M55" s="38"/>
-      <c r="N55" s="17" t="s">
+      <c r="K55" s="21"/>
+      <c r="L55" s="16">
+        <v>4800</v>
+      </c>
+      <c r="M55" s="21">
+        <v>3</v>
+      </c>
+      <c r="N55" s="38"/>
+      <c r="O55" s="17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="56" spans="1:14" ht="20.100000000000001" customHeight="1">
+    <row r="56" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A56" s="3">
         <v>53</v>
       </c>
       <c r="B56" s="41" t="s">
         <v>80</v>
       </c>
-      <c r="C56" s="45"/>
-      <c r="D56" s="45"/>
-      <c r="E56" s="18" t="s">
+      <c r="C56" s="52"/>
+      <c r="D56" s="60" t="s">
+        <v>88</v>
+      </c>
+      <c r="E56" s="45" t="s">
+        <v>174</v>
+      </c>
+      <c r="F56" s="18" t="s">
         <v>142</v>
       </c>
-      <c r="F56" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="G56" s="20" t="s">
+      <c r="G56" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="H56" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="H56" s="27">
+      <c r="I56" s="27">
         <v>127.8</v>
       </c>
-      <c r="I56" s="21"/>
       <c r="J56" s="21"/>
-      <c r="K56" s="16">
-        <v>4800</v>
-      </c>
-      <c r="L56" s="21">
-        <v>3</v>
-      </c>
-      <c r="M56" s="38"/>
-      <c r="N56" s="17" t="s">
+      <c r="K56" s="21"/>
+      <c r="L56" s="16">
+        <v>4800</v>
+      </c>
+      <c r="M56" s="21">
+        <v>3</v>
+      </c>
+      <c r="N56" s="38"/>
+      <c r="O56" s="17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="57" spans="1:14" ht="20.100000000000001" customHeight="1">
+    <row r="57" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A57" s="3">
         <v>54</v>
       </c>
       <c r="B57" s="41" t="s">
         <v>136</v>
       </c>
-      <c r="C57" s="45"/>
-      <c r="D57" s="45"/>
-      <c r="E57" s="18" t="s">
+      <c r="C57" s="52"/>
+      <c r="D57" s="60" t="s">
+        <v>88</v>
+      </c>
+      <c r="E57" s="45" t="s">
+        <v>174</v>
+      </c>
+      <c r="F57" s="18" t="s">
         <v>143</v>
       </c>
-      <c r="F57" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="G57" s="20" t="s">
+      <c r="G57" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="H57" s="20" t="s">
         <v>177</v>
       </c>
-      <c r="H57" s="27">
+      <c r="I57" s="27">
         <v>202.4</v>
       </c>
-      <c r="I57" s="21"/>
       <c r="J57" s="21"/>
-      <c r="K57" s="16">
-        <v>4800</v>
-      </c>
-      <c r="L57" s="21">
-        <v>3</v>
-      </c>
-      <c r="M57" s="38"/>
-      <c r="N57" s="17" t="s">
+      <c r="K57" s="21"/>
+      <c r="L57" s="16">
+        <v>4800</v>
+      </c>
+      <c r="M57" s="21">
+        <v>3</v>
+      </c>
+      <c r="N57" s="38"/>
+      <c r="O57" s="17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="58" spans="1:14" ht="20.100000000000001" customHeight="1">
+    <row r="58" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A58" s="3">
         <v>55</v>
       </c>
       <c r="B58" s="41" t="s">
         <v>137</v>
       </c>
-      <c r="C58" s="45"/>
-      <c r="D58" s="45"/>
-      <c r="E58" s="18" t="s">
+      <c r="C58" s="52"/>
+      <c r="D58" s="60" t="s">
+        <v>88</v>
+      </c>
+      <c r="E58" s="45" t="s">
+        <v>174</v>
+      </c>
+      <c r="F58" s="18" t="s">
         <v>144</v>
       </c>
-      <c r="F58" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="G58" s="20" t="s">
+      <c r="G58" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="H58" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="H58" s="27">
+      <c r="I58" s="27">
         <v>257.31</v>
       </c>
-      <c r="I58" s="21"/>
       <c r="J58" s="21"/>
-      <c r="K58" s="16">
-        <v>4800</v>
-      </c>
-      <c r="L58" s="21">
-        <v>3</v>
-      </c>
-      <c r="M58" s="38"/>
-      <c r="N58" s="17" t="s">
+      <c r="K58" s="21"/>
+      <c r="L58" s="16">
+        <v>4800</v>
+      </c>
+      <c r="M58" s="21">
+        <v>3</v>
+      </c>
+      <c r="N58" s="38"/>
+      <c r="O58" s="17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="59" spans="1:14" ht="20.100000000000001" customHeight="1">
+    <row r="59" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A59" s="3">
         <v>56</v>
       </c>
       <c r="B59" s="41" t="s">
         <v>138</v>
       </c>
-      <c r="C59" s="45"/>
-      <c r="D59" s="45"/>
-      <c r="E59" s="18" t="s">
+      <c r="C59" s="52"/>
+      <c r="D59" s="60" t="s">
+        <v>88</v>
+      </c>
+      <c r="E59" s="45" t="s">
+        <v>174</v>
+      </c>
+      <c r="F59" s="18" t="s">
         <v>145</v>
       </c>
-      <c r="F59" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="G59" s="20" t="s">
+      <c r="G59" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="H59" s="20" t="s">
         <v>153</v>
       </c>
-      <c r="H59" s="28">
+      <c r="I59" s="28">
         <v>1143.71</v>
       </c>
-      <c r="I59" s="21"/>
       <c r="J59" s="21"/>
-      <c r="K59" s="16">
-        <v>4800</v>
-      </c>
-      <c r="L59" s="21">
-        <v>3</v>
-      </c>
-      <c r="M59" s="38"/>
-      <c r="N59" s="17" t="s">
+      <c r="K59" s="21"/>
+      <c r="L59" s="16">
+        <v>4800</v>
+      </c>
+      <c r="M59" s="21">
+        <v>3</v>
+      </c>
+      <c r="N59" s="38"/>
+      <c r="O59" s="17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="60" spans="1:14" ht="20.100000000000001" customHeight="1">
+    <row r="60" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A60" s="3">
         <v>57</v>
       </c>
       <c r="B60" s="41" t="s">
         <v>139</v>
       </c>
-      <c r="C60" s="46"/>
-      <c r="D60" s="46"/>
-      <c r="E60" s="18" t="s">
+      <c r="C60" s="51"/>
+      <c r="D60" s="60" t="s">
+        <v>88</v>
+      </c>
+      <c r="E60" s="45" t="s">
+        <v>174</v>
+      </c>
+      <c r="F60" s="18" t="s">
         <v>146</v>
       </c>
-      <c r="F60" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="G60" s="20" t="s">
+      <c r="G60" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="H60" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="H60" s="27">
+      <c r="I60" s="27">
         <v>31.5</v>
       </c>
-      <c r="I60" s="21"/>
       <c r="J60" s="21"/>
-      <c r="K60" s="16">
-        <v>4800</v>
-      </c>
-      <c r="L60" s="21">
-        <v>3</v>
-      </c>
-      <c r="M60" s="38"/>
-      <c r="N60" s="17" t="s">
+      <c r="K60" s="21"/>
+      <c r="L60" s="16">
+        <v>4800</v>
+      </c>
+      <c r="M60" s="21">
+        <v>3</v>
+      </c>
+      <c r="N60" s="38"/>
+      <c r="O60" s="17" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="A1:P1"/>
+  <mergeCells count="6">
+    <mergeCell ref="C23:C60"/>
+    <mergeCell ref="O2:Q2"/>
+    <mergeCell ref="A2:N2"/>
+    <mergeCell ref="A1:Q1"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:C22"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="D6:D9"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="D12:D22"/>
-    <mergeCell ref="C23:C60"/>
-    <mergeCell ref="D23:D31"/>
-    <mergeCell ref="D32:D36"/>
-    <mergeCell ref="D37:D60"/>
-    <mergeCell ref="N2:P2"/>
-    <mergeCell ref="A2:M2"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.27777800000000002" footer="0.27777800000000002"/>
@@ -4828,7 +5112,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="17.25" customHeight="1">
-      <c r="A2" s="56">
+      <c r="A2" s="58">
         <v>1</v>
       </c>
       <c r="B2" s="5">
@@ -4851,7 +5135,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A3" s="56"/>
+      <c r="A3" s="58"/>
       <c r="B3" s="5">
         <v>1</v>
       </c>
@@ -4872,7 +5156,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="17.25" customHeight="1">
-      <c r="A4" s="56"/>
+      <c r="A4" s="58"/>
       <c r="B4" s="5">
         <v>1</v>
       </c>
@@ -4916,7 +5200,7 @@
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="56">
+      <c r="A6" s="58">
         <v>3</v>
       </c>
       <c r="B6" s="5">
@@ -4939,7 +5223,7 @@
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="56"/>
+      <c r="A7" s="58"/>
       <c r="B7" s="5">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
by Saw Set FlowLayout to zones , groups and floor.
</commit_message>
<xml_diff>
--- a/DataSource/InputData.xlsx
+++ b/DataSource/InputData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Job\Wyzrs\Dev3\Project\DEV-3_Nevron_0601\DEV-3_Nevron_0601\DEV-3_Nevron_0429\DEV-3_Nevron\DataSource\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Job\Wyzrs\Dev3\Project\DEV-3_Nevron_0601\DEV-3_Nevron_0601\DEV-3_Nevron_0601\DEV-3_Nevron_0429\DEV-3_Nevron\DataSource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F32FF8C-E46C-414B-97AD-8F27CBAFEBB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC2973EC-0E38-4206-88A0-961A797DDB17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2634,10 +2634,10 @@
   <dimension ref="A1:Q60"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="3" topLeftCell="E42" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="3" topLeftCell="I4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G41" sqref="G41:G60"/>
+      <selection pane="bottomRight" activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="20.100000000000001" customHeight="1"/>
@@ -2967,7 +2967,7 @@
         <v>4800</v>
       </c>
       <c r="M9" s="21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N9" s="38"/>
       <c r="O9" s="17" t="s">
@@ -3061,7 +3061,7 @@
       </c>
       <c r="C12" s="58"/>
       <c r="D12" s="46" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="E12" s="44" t="s">
         <v>184</v>

</xml_diff>

<commit_message>
by saw lay Change red zones to other color
</commit_message>
<xml_diff>
--- a/DataSource/InputData.xlsx
+++ b/DataSource/InputData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Job\Wyzrs\Dev3\Project\DEV-3_Nevron_0601\DEV-3_Nevron_0601\DEV-3_Nevron_0601\DEV-3_Nevron_0429\DEV-3_Nevron\DataSource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4315FB74-4360-445C-9CA5-8FF7A4C9A91F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F25C8F8F-7929-40C3-A2B1-6D3D9EBB5DDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2629,10 +2629,10 @@
   <dimension ref="A1:Q60"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="3" topLeftCell="H4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J11" sqref="J11"/>
+      <selection pane="bottomRight" activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="20.100000000000001" customHeight="1"/>
@@ -2834,7 +2834,7 @@
         <v>172</v>
       </c>
       <c r="H6" s="20" t="s">
-        <v>145</v>
+        <v>168</v>
       </c>
       <c r="I6" s="25">
         <v>5615.03</v>
@@ -3107,7 +3107,7 @@
         <v>177</v>
       </c>
       <c r="H13" s="20" t="s">
-        <v>145</v>
+        <v>166</v>
       </c>
       <c r="I13" s="26">
         <v>479.52</v>
@@ -4357,7 +4357,7 @@
         <v>184</v>
       </c>
       <c r="H45" s="20" t="s">
-        <v>145</v>
+        <v>165</v>
       </c>
       <c r="I45" s="27">
         <v>59.84</v>
@@ -4903,7 +4903,7 @@
         <v>184</v>
       </c>
       <c r="H59" s="20" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="I59" s="28">
         <v>1143.71</v>

</xml_diff>

<commit_message>
By saw lay -Remove Group color and Area col at DS file and fix in codes for that issues -Change zone red color to other color -continue for H/V connector case
</commit_message>
<xml_diff>
--- a/DataSource/InputData.xlsx
+++ b/DataSource/InputData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Job\Wyzrs\Dev3\Project\DEV-3_Nevron_0601\DEV-3_Nevron_0601\DEV-3_Nevron_0601\DEV-3_Nevron_0429\DEV-3_Nevron\DataSource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4315FB74-4360-445C-9CA5-8FF7A4C9A91F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E74B3D25-0E4A-48C7-95B5-0AE7D123BD8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="Edge" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Input Data_Module'!$A$3:$O$60</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Input Data_Module'!$F$1:$F$60</definedName>
     <definedName name="H">Edge!$P$11:$P$14</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="176">
   <si>
     <t>Purple</t>
   </si>
@@ -744,21 +744,6 @@
     <t>Brown</t>
   </si>
   <si>
-    <t>Group color</t>
-  </si>
-  <si>
-    <t>Group area</t>
-  </si>
-  <si>
-    <t>4800</t>
-  </si>
-  <si>
-    <t>10500</t>
-  </si>
-  <si>
-    <t>8900</t>
-  </si>
-  <si>
     <t>Research Facility</t>
   </si>
   <si>
@@ -768,9 +753,6 @@
     <t>Business Facilities</t>
   </si>
   <si>
-    <t>20000</t>
-  </si>
-  <si>
     <t>Common Use Facility 1</t>
   </si>
   <si>
@@ -781,15 +763,6 @@
   </si>
   <si>
     <t>Public Facilities 1</t>
-  </si>
-  <si>
-    <t>Grey</t>
-  </si>
-  <si>
-    <t>20500</t>
-  </si>
-  <si>
-    <t>24000</t>
   </si>
 </sst>
 </file>
@@ -903,7 +876,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="31">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -928,21 +901,6 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="11"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="11"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color indexed="10"/>
       </left>
       <right style="thin">
@@ -950,21 +908,6 @@
       </right>
       <top style="thin">
         <color indexed="11"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="11"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
       </top>
       <bottom style="thin">
         <color indexed="10"/>
@@ -1287,7 +1230,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1297,10 +1240,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1309,16 +1252,16 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1327,10 +1270,19 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
@@ -1339,55 +1291,40 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="9" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="9" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="4" fontId="9" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="9" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
@@ -1396,73 +1333,67 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="20" fontId="2" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="2" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2626,2346 +2557,1994 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:Q60"/>
+  <dimension ref="A1:O60"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="3" topLeftCell="H4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J11" sqref="J11"/>
+      <selection pane="bottomRight" activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="20.100000000000001" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="6.88671875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.88671875" style="43" customWidth="1"/>
+    <col min="2" max="2" width="16.88671875" style="41" customWidth="1"/>
     <col min="3" max="3" width="12" style="1" customWidth="1"/>
-    <col min="4" max="5" width="20" style="1" customWidth="1"/>
-    <col min="6" max="6" width="13.44140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12" style="1" customWidth="1"/>
-    <col min="8" max="8" width="20" style="1" customWidth="1"/>
-    <col min="9" max="17" width="16.33203125" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="16.33203125" style="1"/>
+    <col min="4" max="4" width="20" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.44140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="20" style="1" customWidth="1"/>
+    <col min="7" max="15" width="16.33203125" style="1" customWidth="1"/>
+    <col min="16" max="16384" width="16.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="27.6" customHeight="1">
-      <c r="A1" s="55" t="s">
+    <row r="1" spans="1:15" ht="27.6" customHeight="1">
+      <c r="A1" s="51" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55"/>
-      <c r="H1" s="55"/>
-      <c r="I1" s="55"/>
-      <c r="J1" s="55"/>
-      <c r="K1" s="55"/>
-      <c r="L1" s="55"/>
-      <c r="M1" s="55"/>
-      <c r="N1" s="55"/>
-      <c r="O1" s="55"/>
-      <c r="P1" s="55"/>
-      <c r="Q1" s="55"/>
-    </row>
-    <row r="2" spans="1:17" ht="24" customHeight="1">
-      <c r="A2" s="53"/>
-      <c r="B2" s="53"/>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="53"/>
-      <c r="I2" s="53"/>
-      <c r="J2" s="53"/>
-      <c r="K2" s="53"/>
-      <c r="L2" s="53"/>
-      <c r="M2" s="53"/>
-      <c r="N2" s="54"/>
-      <c r="O2" s="50"/>
-      <c r="P2" s="51"/>
-      <c r="Q2" s="52"/>
-    </row>
-    <row r="3" spans="1:17" ht="20.25" customHeight="1" thickBot="1">
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="51"/>
+      <c r="J1" s="51"/>
+      <c r="K1" s="51"/>
+      <c r="L1" s="51"/>
+      <c r="M1" s="51"/>
+      <c r="N1" s="51"/>
+      <c r="O1" s="51"/>
+    </row>
+    <row r="2" spans="1:15" ht="24" customHeight="1">
+      <c r="A2" s="49"/>
+      <c r="B2" s="49"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49"/>
+      <c r="K2" s="49"/>
+      <c r="L2" s="50"/>
+      <c r="M2" s="46"/>
+      <c r="N2" s="47"/>
+      <c r="O2" s="48"/>
+    </row>
+    <row r="3" spans="1:15" ht="20.25" customHeight="1" thickBot="1">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="39" t="s">
+      <c r="B3" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="56" t="s">
+      <c r="C3" s="52" t="s">
         <v>141</v>
       </c>
-      <c r="D3" s="56"/>
-      <c r="E3" s="45" t="s">
-        <v>169</v>
-      </c>
-      <c r="F3" s="7" t="s">
+      <c r="D3" s="52"/>
+      <c r="E3" s="7" t="s">
         <v>30</v>
       </c>
+      <c r="F3" s="8" t="s">
+        <v>31</v>
+      </c>
       <c r="G3" s="8" t="s">
-        <v>170</v>
+        <v>142</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>142</v>
+        <v>33</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="K3" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="L3" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="M3" s="9" t="s">
+      <c r="K3" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="N3" s="36" t="s">
+      <c r="L3" s="34" t="s">
         <v>164</v>
       </c>
-      <c r="O3" s="10" t="s">
+      <c r="M3" s="10" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="20.25" customHeight="1" thickTop="1">
+    <row r="4" spans="1:15" ht="20.25" customHeight="1" thickTop="1">
       <c r="A4" s="3">
         <v>1</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="C4" s="57" t="s">
+      <c r="C4" s="53" t="s">
         <v>84</v>
       </c>
-      <c r="D4" s="46" t="s">
-        <v>174</v>
-      </c>
-      <c r="E4" s="44" t="s">
-        <v>182</v>
-      </c>
-      <c r="F4" s="13" t="s">
+      <c r="D4" s="42" t="s">
+        <v>169</v>
+      </c>
+      <c r="E4" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="14" t="s">
-        <v>171</v>
-      </c>
-      <c r="H4" s="15" t="s">
+      <c r="F4" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="I4" s="24">
+      <c r="G4" s="22">
         <v>805.12</v>
       </c>
-      <c r="J4" s="16"/>
-      <c r="K4" s="16"/>
-      <c r="L4" s="16">
-        <v>4800</v>
-      </c>
-      <c r="M4" s="16">
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15">
+        <v>4800</v>
+      </c>
+      <c r="K4" s="15">
         <v>1</v>
       </c>
-      <c r="N4" s="37"/>
-      <c r="O4" s="17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" ht="20.100000000000001" customHeight="1">
+      <c r="L4" s="35"/>
+      <c r="M4" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A5" s="3">
         <v>2</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="C5" s="58"/>
-      <c r="D5" s="46" t="s">
-        <v>174</v>
-      </c>
-      <c r="E5" s="44" t="s">
-        <v>182</v>
+      <c r="C5" s="54"/>
+      <c r="D5" s="42" t="s">
+        <v>169</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>2</v>
       </c>
       <c r="F5" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="G5" s="14" t="s">
-        <v>171</v>
-      </c>
-      <c r="H5" s="20" t="s">
         <v>167</v>
       </c>
-      <c r="I5" s="25">
+      <c r="G5" s="23">
         <v>3983.44</v>
       </c>
-      <c r="J5" s="21"/>
-      <c r="K5" s="21"/>
-      <c r="L5" s="16">
-        <v>4800</v>
-      </c>
-      <c r="M5" s="21">
+      <c r="H5" s="19"/>
+      <c r="I5" s="19"/>
+      <c r="J5" s="15">
+        <v>4800</v>
+      </c>
+      <c r="K5" s="19">
         <v>1</v>
       </c>
-      <c r="N5" s="38"/>
-      <c r="O5" s="17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" ht="20.100000000000001" customHeight="1">
+      <c r="L5" s="36"/>
+      <c r="M5" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A6" s="3">
         <v>3</v>
       </c>
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="C6" s="58"/>
-      <c r="D6" s="46" t="s">
-        <v>175</v>
-      </c>
-      <c r="E6" s="44" t="s">
-        <v>182</v>
+      <c r="C6" s="54"/>
+      <c r="D6" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>21</v>
       </c>
       <c r="F6" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="G6" s="19" t="s">
-        <v>172</v>
-      </c>
-      <c r="H6" s="20" t="s">
-        <v>145</v>
-      </c>
-      <c r="I6" s="25">
+        <v>146</v>
+      </c>
+      <c r="G6" s="23">
         <v>5615.03</v>
       </c>
-      <c r="J6" s="21"/>
-      <c r="K6" s="21"/>
-      <c r="L6" s="16">
-        <v>4800</v>
-      </c>
-      <c r="M6" s="21">
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="15">
+        <v>4800</v>
+      </c>
+      <c r="K6" s="19">
         <v>1</v>
       </c>
-      <c r="N6" s="38"/>
-      <c r="O6" s="17" t="s">
+      <c r="L6" s="36"/>
+      <c r="M6" s="16" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="20.85" customHeight="1">
+    <row r="7" spans="1:15" ht="20.85" customHeight="1">
       <c r="A7" s="4">
         <v>4</v>
       </c>
-      <c r="B7" s="23" t="s">
+      <c r="B7" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="C7" s="58"/>
-      <c r="D7" s="46" t="s">
-        <v>175</v>
-      </c>
-      <c r="E7" s="44" t="s">
-        <v>182</v>
+      <c r="C7" s="54"/>
+      <c r="D7" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>3</v>
       </c>
       <c r="F7" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="G7" s="19" t="s">
-        <v>172</v>
-      </c>
-      <c r="H7" s="20" t="s">
-        <v>146</v>
-      </c>
-      <c r="I7" s="25">
+        <v>168</v>
+      </c>
+      <c r="G7" s="23">
         <v>1885.68</v>
       </c>
-      <c r="J7" s="21"/>
-      <c r="K7" s="21"/>
-      <c r="L7" s="16">
-        <v>4800</v>
-      </c>
-      <c r="M7" s="21">
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="15">
+        <v>4800</v>
+      </c>
+      <c r="K7" s="19">
         <v>1</v>
       </c>
-      <c r="N7" s="38"/>
-      <c r="O7" s="17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" ht="20.100000000000001" customHeight="1">
+      <c r="L7" s="36"/>
+      <c r="M7" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A8" s="4">
         <v>5</v>
       </c>
-      <c r="B8" s="23" t="s">
+      <c r="B8" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="C8" s="58"/>
-      <c r="D8" s="46" t="s">
-        <v>175</v>
-      </c>
-      <c r="E8" s="44" t="s">
-        <v>182</v>
+      <c r="C8" s="54"/>
+      <c r="D8" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>4</v>
       </c>
       <c r="F8" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="G8" s="19" t="s">
-        <v>172</v>
-      </c>
-      <c r="H8" s="20" t="s">
         <v>165</v>
       </c>
-      <c r="I8" s="25">
+      <c r="G8" s="23">
         <v>2495.8000000000002</v>
       </c>
-      <c r="J8" s="21"/>
-      <c r="K8" s="21"/>
-      <c r="L8" s="16">
-        <v>4800</v>
-      </c>
-      <c r="M8" s="21">
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="15">
+        <v>4800</v>
+      </c>
+      <c r="K8" s="19">
         <v>1</v>
       </c>
-      <c r="N8" s="38"/>
-      <c r="O8" s="17" t="s">
+      <c r="L8" s="36"/>
+      <c r="M8" s="16" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="20.100000000000001" customHeight="1">
+    <row r="9" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A9" s="3">
         <v>6</v>
       </c>
-      <c r="B9" s="23" t="s">
+      <c r="B9" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="C9" s="58"/>
-      <c r="D9" s="46" t="s">
-        <v>175</v>
-      </c>
-      <c r="E9" s="44" t="s">
-        <v>182</v>
+      <c r="C9" s="54"/>
+      <c r="D9" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>5</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="G9" s="19" t="s">
-        <v>172</v>
-      </c>
-      <c r="H9" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="I9" s="26">
+      <c r="G9" s="24">
         <v>475.39</v>
       </c>
-      <c r="J9" s="21"/>
-      <c r="K9" s="21"/>
-      <c r="L9" s="16">
-        <v>4800</v>
-      </c>
-      <c r="M9" s="21">
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="15">
+        <v>4800</v>
+      </c>
+      <c r="K9" s="19">
         <v>1</v>
       </c>
-      <c r="N9" s="38"/>
-      <c r="O9" s="17" t="s">
+      <c r="L9" s="36"/>
+      <c r="M9" s="16" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="20.100000000000001" customHeight="1">
+    <row r="10" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A10" s="3">
         <v>7</v>
       </c>
-      <c r="B10" s="23" t="s">
+      <c r="B10" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="C10" s="58"/>
-      <c r="D10" s="46" t="s">
-        <v>181</v>
-      </c>
-      <c r="E10" s="44" t="s">
-        <v>182</v>
+      <c r="C10" s="54"/>
+      <c r="D10" s="42" t="s">
+        <v>175</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>6</v>
       </c>
       <c r="F10" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="G10" s="19" t="s">
-        <v>173</v>
-      </c>
-      <c r="H10" s="20" t="s">
         <v>165</v>
       </c>
-      <c r="I10" s="25">
+      <c r="G10" s="23">
         <v>7368</v>
       </c>
-      <c r="J10" s="21"/>
-      <c r="K10" s="21"/>
-      <c r="L10" s="16">
-        <v>4800</v>
-      </c>
-      <c r="M10" s="21">
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="15">
+        <v>4800</v>
+      </c>
+      <c r="K10" s="19">
         <v>2</v>
       </c>
-      <c r="N10" s="38"/>
-      <c r="O10" s="17" t="s">
+      <c r="L10" s="36"/>
+      <c r="M10" s="16" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="20.100000000000001" customHeight="1">
+    <row r="11" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A11" s="3">
         <v>8</v>
       </c>
-      <c r="B11" s="23" t="s">
+      <c r="B11" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="C11" s="58"/>
-      <c r="D11" s="46" t="s">
-        <v>181</v>
-      </c>
-      <c r="E11" s="44" t="s">
-        <v>182</v>
+      <c r="C11" s="54"/>
+      <c r="D11" s="42" t="s">
+        <v>175</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>4</v>
       </c>
       <c r="F11" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="G11" s="19" t="s">
-        <v>173</v>
-      </c>
-      <c r="H11" s="20" t="s">
         <v>166</v>
       </c>
-      <c r="I11" s="25">
+      <c r="G11" s="23">
         <v>1499.07</v>
       </c>
-      <c r="J11" s="21"/>
-      <c r="K11" s="21"/>
-      <c r="L11" s="16">
-        <v>4800</v>
-      </c>
-      <c r="M11" s="21">
+      <c r="H11" s="19"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="15">
+        <v>4800</v>
+      </c>
+      <c r="K11" s="19">
         <v>2</v>
       </c>
-      <c r="N11" s="38"/>
-      <c r="O11" s="17" t="s">
+      <c r="L11" s="36"/>
+      <c r="M11" s="16" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="20.100000000000001" customHeight="1">
+    <row r="12" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A12" s="3">
         <v>9</v>
       </c>
-      <c r="B12" s="23" t="s">
+      <c r="B12" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="C12" s="58"/>
-      <c r="D12" s="46" t="s">
-        <v>181</v>
-      </c>
-      <c r="E12" s="44" t="s">
-        <v>182</v>
+      <c r="C12" s="54"/>
+      <c r="D12" s="42" t="s">
+        <v>175</v>
+      </c>
+      <c r="E12" s="17" t="s">
+        <v>7</v>
       </c>
       <c r="F12" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="G12" s="19" t="s">
-        <v>177</v>
-      </c>
-      <c r="H12" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="I12" s="26">
+      <c r="G12" s="24">
         <v>322.32</v>
       </c>
-      <c r="J12" s="21"/>
-      <c r="K12" s="21"/>
-      <c r="L12" s="16">
-        <v>4800</v>
-      </c>
-      <c r="M12" s="21">
+      <c r="H12" s="19"/>
+      <c r="I12" s="19"/>
+      <c r="J12" s="15">
+        <v>4800</v>
+      </c>
+      <c r="K12" s="19">
         <v>2</v>
       </c>
-      <c r="N12" s="38"/>
-      <c r="O12" s="17" t="s">
+      <c r="L12" s="36"/>
+      <c r="M12" s="16" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="20.100000000000001" customHeight="1">
+    <row r="13" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A13" s="3">
         <v>10</v>
       </c>
-      <c r="B13" s="23" t="s">
+      <c r="B13" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="C13" s="58"/>
-      <c r="D13" s="46" t="s">
-        <v>178</v>
-      </c>
-      <c r="E13" s="44" t="s">
-        <v>182</v>
+      <c r="C13" s="54"/>
+      <c r="D13" s="42" t="s">
+        <v>172</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>8</v>
       </c>
       <c r="F13" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="G13" s="19" t="s">
-        <v>177</v>
-      </c>
-      <c r="H13" s="20" t="s">
-        <v>145</v>
-      </c>
-      <c r="I13" s="26">
+        <v>167</v>
+      </c>
+      <c r="G13" s="24">
         <v>479.52</v>
       </c>
-      <c r="J13" s="21"/>
-      <c r="K13" s="21"/>
-      <c r="L13" s="16">
-        <v>4800</v>
-      </c>
-      <c r="M13" s="21">
-        <v>3</v>
-      </c>
-      <c r="N13" s="38"/>
-      <c r="O13" s="17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" ht="20.100000000000001" customHeight="1">
+      <c r="H13" s="19"/>
+      <c r="I13" s="19"/>
+      <c r="J13" s="15">
+        <v>4800</v>
+      </c>
+      <c r="K13" s="19">
+        <v>3</v>
+      </c>
+      <c r="L13" s="36"/>
+      <c r="M13" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A14" s="3">
         <v>11</v>
       </c>
-      <c r="B14" s="23" t="s">
+      <c r="B14" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="C14" s="58"/>
-      <c r="D14" s="46" t="s">
-        <v>178</v>
-      </c>
-      <c r="E14" s="44" t="s">
-        <v>182</v>
+      <c r="C14" s="54"/>
+      <c r="D14" s="42" t="s">
+        <v>172</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>49</v>
       </c>
       <c r="F14" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="G14" s="19" t="s">
-        <v>177</v>
-      </c>
-      <c r="H14" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="I14" s="26">
+      <c r="G14" s="24">
         <v>195.84</v>
       </c>
-      <c r="J14" s="21"/>
-      <c r="K14" s="21"/>
-      <c r="L14" s="16">
-        <v>4800</v>
-      </c>
-      <c r="M14" s="21">
-        <v>3</v>
-      </c>
-      <c r="N14" s="38"/>
-      <c r="O14" s="17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" ht="20.100000000000001" customHeight="1">
+      <c r="H14" s="19"/>
+      <c r="I14" s="19"/>
+      <c r="J14" s="15">
+        <v>4800</v>
+      </c>
+      <c r="K14" s="19">
+        <v>3</v>
+      </c>
+      <c r="L14" s="36"/>
+      <c r="M14" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A15" s="3">
         <v>12</v>
       </c>
-      <c r="B15" s="23" t="s">
+      <c r="B15" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="C15" s="58"/>
-      <c r="D15" s="46" t="s">
-        <v>178</v>
-      </c>
-      <c r="E15" s="44" t="s">
-        <v>182</v>
+      <c r="C15" s="54"/>
+      <c r="D15" s="42" t="s">
+        <v>172</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>6</v>
       </c>
       <c r="F15" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="G15" s="19" t="s">
-        <v>177</v>
-      </c>
-      <c r="H15" s="20" t="s">
         <v>165</v>
       </c>
-      <c r="I15" s="26">
+      <c r="G15" s="24">
         <v>139.12</v>
       </c>
-      <c r="J15" s="21"/>
-      <c r="K15" s="21"/>
-      <c r="L15" s="16">
-        <v>4800</v>
-      </c>
-      <c r="M15" s="21">
-        <v>3</v>
-      </c>
-      <c r="N15" s="38"/>
-      <c r="O15" s="17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" ht="20.100000000000001" customHeight="1">
+      <c r="H15" s="19"/>
+      <c r="I15" s="19"/>
+      <c r="J15" s="15">
+        <v>4800</v>
+      </c>
+      <c r="K15" s="19">
+        <v>3</v>
+      </c>
+      <c r="L15" s="36"/>
+      <c r="M15" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A16" s="3">
         <v>13</v>
       </c>
-      <c r="B16" s="23" t="s">
+      <c r="B16" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="C16" s="58"/>
-      <c r="D16" s="46" t="s">
-        <v>178</v>
-      </c>
-      <c r="E16" s="44" t="s">
-        <v>182</v>
+      <c r="C16" s="54"/>
+      <c r="D16" s="42" t="s">
+        <v>172</v>
+      </c>
+      <c r="E16" s="17" t="s">
+        <v>4</v>
       </c>
       <c r="F16" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="G16" s="19" t="s">
-        <v>177</v>
-      </c>
-      <c r="H16" s="20" t="s">
         <v>168</v>
       </c>
-      <c r="I16" s="26">
+      <c r="G16" s="24">
         <v>391.68</v>
       </c>
-      <c r="J16" s="21"/>
-      <c r="K16" s="21"/>
-      <c r="L16" s="16">
-        <v>4800</v>
-      </c>
-      <c r="M16" s="21">
-        <v>3</v>
-      </c>
-      <c r="N16" s="38"/>
-      <c r="O16" s="17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" ht="20.100000000000001" customHeight="1">
+      <c r="H16" s="19"/>
+      <c r="I16" s="19"/>
+      <c r="J16" s="15">
+        <v>4800</v>
+      </c>
+      <c r="K16" s="19">
+        <v>3</v>
+      </c>
+      <c r="L16" s="36"/>
+      <c r="M16" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="20.100000000000001" customHeight="1">
       <c r="A17" s="3">
         <v>14</v>
       </c>
-      <c r="B17" s="23" t="s">
+      <c r="B17" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="C17" s="58"/>
-      <c r="D17" s="46" t="s">
-        <v>178</v>
-      </c>
-      <c r="E17" s="44" t="s">
-        <v>182</v>
+      <c r="C17" s="54"/>
+      <c r="D17" s="42" t="s">
+        <v>172</v>
+      </c>
+      <c r="E17" s="17" t="s">
+        <v>50</v>
       </c>
       <c r="F17" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="G17" s="19" t="s">
-        <v>177</v>
-      </c>
-      <c r="H17" s="20" t="s">
         <v>146</v>
       </c>
-      <c r="I17" s="26">
+      <c r="G17" s="24">
         <v>97.92</v>
       </c>
-      <c r="J17" s="21"/>
-      <c r="K17" s="21"/>
-      <c r="L17" s="16">
-        <v>4800</v>
-      </c>
-      <c r="M17" s="21">
-        <v>3</v>
-      </c>
-      <c r="N17" s="38"/>
-      <c r="O17" s="17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" ht="20.100000000000001" customHeight="1">
+      <c r="H17" s="19"/>
+      <c r="I17" s="19"/>
+      <c r="J17" s="15">
+        <v>4800</v>
+      </c>
+      <c r="K17" s="19">
+        <v>3</v>
+      </c>
+      <c r="L17" s="36"/>
+      <c r="M17" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="20.100000000000001" customHeight="1">
       <c r="A18" s="3">
         <v>15</v>
       </c>
-      <c r="B18" s="23" t="s">
+      <c r="B18" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="C18" s="58"/>
-      <c r="D18" s="46" t="s">
-        <v>178</v>
-      </c>
-      <c r="E18" s="44" t="s">
-        <v>182</v>
+      <c r="C18" s="54"/>
+      <c r="D18" s="42" t="s">
+        <v>172</v>
+      </c>
+      <c r="E18" s="17" t="s">
+        <v>51</v>
       </c>
       <c r="F18" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="G18" s="19" t="s">
-        <v>177</v>
-      </c>
-      <c r="H18" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="I18" s="26">
+      <c r="G18" s="24">
         <v>391.68</v>
       </c>
-      <c r="J18" s="21"/>
-      <c r="K18" s="21"/>
-      <c r="L18" s="16">
-        <v>4800</v>
-      </c>
-      <c r="M18" s="21">
-        <v>3</v>
-      </c>
-      <c r="N18" s="38"/>
-      <c r="O18" s="17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" ht="20.100000000000001" customHeight="1">
+      <c r="H18" s="19"/>
+      <c r="I18" s="19"/>
+      <c r="J18" s="15">
+        <v>4800</v>
+      </c>
+      <c r="K18" s="19">
+        <v>3</v>
+      </c>
+      <c r="L18" s="36"/>
+      <c r="M18" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="20.100000000000001" customHeight="1">
       <c r="A19" s="3">
         <v>16</v>
       </c>
-      <c r="B19" s="23" t="s">
+      <c r="B19" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="C19" s="58"/>
-      <c r="D19" s="46" t="s">
-        <v>178</v>
-      </c>
-      <c r="E19" s="44" t="s">
-        <v>182</v>
+      <c r="C19" s="54"/>
+      <c r="D19" s="42" t="s">
+        <v>172</v>
+      </c>
+      <c r="E19" s="17" t="s">
+        <v>7</v>
       </c>
       <c r="F19" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="G19" s="19" t="s">
-        <v>177</v>
-      </c>
-      <c r="H19" s="20" t="s">
         <v>146</v>
       </c>
-      <c r="I19" s="26">
+      <c r="G19" s="24">
         <v>781.21</v>
       </c>
-      <c r="J19" s="21"/>
-      <c r="K19" s="21"/>
-      <c r="L19" s="16">
-        <v>4800</v>
-      </c>
-      <c r="M19" s="21">
-        <v>3</v>
-      </c>
-      <c r="N19" s="38"/>
-      <c r="O19" s="17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" ht="20.100000000000001" customHeight="1">
+      <c r="H19" s="19"/>
+      <c r="I19" s="19"/>
+      <c r="J19" s="15">
+        <v>4800</v>
+      </c>
+      <c r="K19" s="19">
+        <v>3</v>
+      </c>
+      <c r="L19" s="36"/>
+      <c r="M19" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="20.100000000000001" customHeight="1">
       <c r="A20" s="3">
         <v>17</v>
       </c>
-      <c r="B20" s="23" t="s">
+      <c r="B20" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="C20" s="58"/>
-      <c r="D20" s="46" t="s">
-        <v>178</v>
-      </c>
-      <c r="E20" s="44" t="s">
-        <v>182</v>
+      <c r="C20" s="54"/>
+      <c r="D20" s="42" t="s">
+        <v>172</v>
+      </c>
+      <c r="E20" s="17" t="s">
+        <v>52</v>
       </c>
       <c r="F20" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="G20" s="19" t="s">
-        <v>177</v>
-      </c>
-      <c r="H20" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="I20" s="26">
+      <c r="G20" s="24">
         <v>541.44000000000005</v>
       </c>
-      <c r="J20" s="21"/>
-      <c r="K20" s="21"/>
-      <c r="L20" s="16">
-        <v>4800</v>
-      </c>
-      <c r="M20" s="21">
-        <v>3</v>
-      </c>
-      <c r="N20" s="38"/>
-      <c r="O20" s="17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" ht="20.100000000000001" customHeight="1">
+      <c r="H20" s="19"/>
+      <c r="I20" s="19"/>
+      <c r="J20" s="15">
+        <v>4800</v>
+      </c>
+      <c r="K20" s="19">
+        <v>3</v>
+      </c>
+      <c r="L20" s="36"/>
+      <c r="M20" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="20.100000000000001" customHeight="1">
       <c r="A21" s="3">
         <v>18</v>
       </c>
-      <c r="B21" s="29" t="s">
+      <c r="B21" s="27" t="s">
         <v>82</v>
       </c>
-      <c r="C21" s="58"/>
-      <c r="D21" s="46" t="s">
-        <v>178</v>
-      </c>
-      <c r="E21" s="44" t="s">
-        <v>182</v>
+      <c r="C21" s="54"/>
+      <c r="D21" s="42" t="s">
+        <v>172</v>
+      </c>
+      <c r="E21" s="17" t="s">
+        <v>53</v>
       </c>
       <c r="F21" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="G21" s="19" t="s">
-        <v>177</v>
-      </c>
-      <c r="H21" s="20" t="s">
         <v>167</v>
       </c>
-      <c r="I21" s="31">
+      <c r="G21" s="29">
         <v>881.61</v>
       </c>
-      <c r="J21" s="21"/>
-      <c r="K21" s="21"/>
-      <c r="L21" s="16">
-        <v>4800</v>
-      </c>
-      <c r="M21" s="21">
-        <v>3</v>
-      </c>
-      <c r="N21" s="38"/>
-      <c r="O21" s="17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" ht="20.100000000000001" customHeight="1">
+      <c r="H21" s="19"/>
+      <c r="I21" s="19"/>
+      <c r="J21" s="15">
+        <v>4800</v>
+      </c>
+      <c r="K21" s="19">
+        <v>3</v>
+      </c>
+      <c r="L21" s="36"/>
+      <c r="M21" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="20.100000000000001" customHeight="1">
       <c r="A22" s="3">
         <v>19</v>
       </c>
-      <c r="B22" s="30" t="s">
+      <c r="B22" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="C22" s="58"/>
-      <c r="D22" s="46" t="s">
-        <v>178</v>
-      </c>
-      <c r="E22" s="44" t="s">
-        <v>182</v>
+      <c r="C22" s="54"/>
+      <c r="D22" s="42" t="s">
+        <v>172</v>
+      </c>
+      <c r="E22" s="17" t="s">
+        <v>54</v>
       </c>
       <c r="F22" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="G22" s="19" t="s">
-        <v>177</v>
-      </c>
-      <c r="H22" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="I22" s="33">
+      <c r="G22" s="31">
         <v>100.64</v>
       </c>
-      <c r="J22" s="21"/>
-      <c r="K22" s="21"/>
-      <c r="L22" s="16">
-        <v>4800</v>
-      </c>
-      <c r="M22" s="21">
-        <v>3</v>
-      </c>
-      <c r="N22" s="38"/>
-      <c r="O22" s="17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" ht="20.100000000000001" customHeight="1">
+      <c r="H22" s="19"/>
+      <c r="I22" s="19"/>
+      <c r="J22" s="15">
+        <v>4800</v>
+      </c>
+      <c r="K22" s="19">
+        <v>3</v>
+      </c>
+      <c r="L22" s="36"/>
+      <c r="M22" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="20.100000000000001" customHeight="1">
       <c r="A23" s="3">
         <v>20</v>
       </c>
-      <c r="B23" s="40" t="s">
+      <c r="B23" s="38" t="s">
         <v>100</v>
       </c>
-      <c r="C23" s="47" t="s">
+      <c r="C23" s="43" t="s">
         <v>140</v>
       </c>
-      <c r="D23" s="46" t="s">
-        <v>176</v>
-      </c>
-      <c r="E23" s="44" t="s">
-        <v>182</v>
+      <c r="D23" s="42" t="s">
+        <v>171</v>
+      </c>
+      <c r="E23" s="17" t="s">
+        <v>55</v>
       </c>
       <c r="F23" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="G23" s="19" t="s">
-        <v>172</v>
-      </c>
-      <c r="H23" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="I23" s="32">
+      <c r="G23" s="30">
         <v>99</v>
       </c>
-      <c r="J23" s="21"/>
-      <c r="K23" s="21"/>
-      <c r="L23" s="16">
-        <v>4800</v>
-      </c>
-      <c r="M23" s="21">
-        <v>3</v>
-      </c>
-      <c r="N23" s="38"/>
-      <c r="O23" s="17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" ht="20.100000000000001" customHeight="1">
+      <c r="H23" s="19"/>
+      <c r="I23" s="19"/>
+      <c r="J23" s="15">
+        <v>4800</v>
+      </c>
+      <c r="K23" s="19">
+        <v>3</v>
+      </c>
+      <c r="L23" s="36"/>
+      <c r="M23" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="20.100000000000001" customHeight="1">
       <c r="A24" s="3">
         <v>21</v>
       </c>
-      <c r="B24" s="41" t="s">
+      <c r="B24" s="39" t="s">
         <v>101</v>
       </c>
-      <c r="C24" s="48"/>
-      <c r="D24" s="46" t="s">
-        <v>176</v>
-      </c>
-      <c r="E24" s="44" t="s">
-        <v>182</v>
+      <c r="C24" s="44"/>
+      <c r="D24" s="42" t="s">
+        <v>171</v>
+      </c>
+      <c r="E24" s="17" t="s">
+        <v>56</v>
       </c>
       <c r="F24" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="G24" s="19" t="s">
-        <v>172</v>
-      </c>
-      <c r="H24" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="I24" s="27">
+      <c r="G24" s="25">
         <v>99</v>
       </c>
-      <c r="J24" s="21"/>
-      <c r="K24" s="21"/>
-      <c r="L24" s="16">
-        <v>4800</v>
-      </c>
-      <c r="M24" s="21">
-        <v>3</v>
-      </c>
-      <c r="N24" s="38"/>
-      <c r="O24" s="17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" ht="20.100000000000001" customHeight="1">
+      <c r="H24" s="19"/>
+      <c r="I24" s="19"/>
+      <c r="J24" s="15">
+        <v>4800</v>
+      </c>
+      <c r="K24" s="19">
+        <v>3</v>
+      </c>
+      <c r="L24" s="36"/>
+      <c r="M24" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="20.100000000000001" customHeight="1">
       <c r="A25" s="3">
         <v>22</v>
       </c>
-      <c r="B25" s="41" t="s">
+      <c r="B25" s="39" t="s">
         <v>102</v>
       </c>
-      <c r="C25" s="48"/>
-      <c r="D25" s="46" t="s">
-        <v>176</v>
-      </c>
-      <c r="E25" s="44" t="s">
-        <v>182</v>
+      <c r="C25" s="44"/>
+      <c r="D25" s="42" t="s">
+        <v>171</v>
+      </c>
+      <c r="E25" s="17" t="s">
+        <v>57</v>
       </c>
       <c r="F25" s="18" t="s">
-        <v>57</v>
-      </c>
-      <c r="G25" s="19" t="s">
-        <v>172</v>
-      </c>
-      <c r="H25" s="20" t="s">
         <v>146</v>
       </c>
-      <c r="I25" s="27">
+      <c r="G25" s="25">
         <v>66</v>
       </c>
-      <c r="J25" s="21"/>
-      <c r="K25" s="21"/>
-      <c r="L25" s="16">
-        <v>4800</v>
-      </c>
-      <c r="M25" s="21">
-        <v>3</v>
-      </c>
-      <c r="N25" s="38"/>
-      <c r="O25" s="17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" ht="20.100000000000001" customHeight="1">
+      <c r="H25" s="19"/>
+      <c r="I25" s="19"/>
+      <c r="J25" s="15">
+        <v>4800</v>
+      </c>
+      <c r="K25" s="19">
+        <v>3</v>
+      </c>
+      <c r="L25" s="36"/>
+      <c r="M25" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="20.100000000000001" customHeight="1">
       <c r="A26" s="3">
         <v>23</v>
       </c>
-      <c r="B26" s="41" t="s">
+      <c r="B26" s="39" t="s">
         <v>103</v>
       </c>
-      <c r="C26" s="48"/>
-      <c r="D26" s="46" t="s">
-        <v>176</v>
-      </c>
-      <c r="E26" s="44" t="s">
-        <v>182</v>
+      <c r="C26" s="44"/>
+      <c r="D26" s="42" t="s">
+        <v>171</v>
+      </c>
+      <c r="E26" s="17" t="s">
+        <v>58</v>
       </c>
       <c r="F26" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="G26" s="19" t="s">
-        <v>172</v>
-      </c>
-      <c r="H26" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="I26" s="27">
+      <c r="G26" s="25">
         <v>66</v>
       </c>
-      <c r="J26" s="21"/>
-      <c r="K26" s="21"/>
-      <c r="L26" s="16">
-        <v>4800</v>
-      </c>
-      <c r="M26" s="21">
-        <v>3</v>
-      </c>
-      <c r="N26" s="38"/>
-      <c r="O26" s="17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" ht="20.100000000000001" customHeight="1">
+      <c r="H26" s="19"/>
+      <c r="I26" s="19"/>
+      <c r="J26" s="15">
+        <v>4800</v>
+      </c>
+      <c r="K26" s="19">
+        <v>3</v>
+      </c>
+      <c r="L26" s="36"/>
+      <c r="M26" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="20.100000000000001" customHeight="1">
       <c r="A27" s="3">
         <v>24</v>
       </c>
-      <c r="B27" s="41" t="s">
+      <c r="B27" s="39" t="s">
         <v>104</v>
       </c>
-      <c r="C27" s="48"/>
-      <c r="D27" s="46" t="s">
-        <v>176</v>
-      </c>
-      <c r="E27" s="44" t="s">
-        <v>182</v>
+      <c r="C27" s="44"/>
+      <c r="D27" s="42" t="s">
+        <v>171</v>
+      </c>
+      <c r="E27" s="17" t="s">
+        <v>59</v>
       </c>
       <c r="F27" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="G27" s="19" t="s">
-        <v>172</v>
-      </c>
-      <c r="H27" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="I27" s="27">
+      <c r="G27" s="25">
         <v>415.87</v>
       </c>
-      <c r="J27" s="21"/>
-      <c r="K27" s="21"/>
-      <c r="L27" s="16">
-        <v>4800</v>
-      </c>
-      <c r="M27" s="21">
-        <v>3</v>
-      </c>
-      <c r="N27" s="38"/>
-      <c r="O27" s="17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" ht="20.100000000000001" customHeight="1">
+      <c r="H27" s="19"/>
+      <c r="I27" s="19"/>
+      <c r="J27" s="15">
+        <v>4800</v>
+      </c>
+      <c r="K27" s="19">
+        <v>3</v>
+      </c>
+      <c r="L27" s="36"/>
+      <c r="M27" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="20.100000000000001" customHeight="1">
       <c r="A28" s="3">
         <v>25</v>
       </c>
-      <c r="B28" s="41" t="s">
+      <c r="B28" s="39" t="s">
         <v>105</v>
       </c>
-      <c r="C28" s="48"/>
-      <c r="D28" s="46" t="s">
-        <v>176</v>
-      </c>
-      <c r="E28" s="44" t="s">
-        <v>182</v>
+      <c r="C28" s="44"/>
+      <c r="D28" s="42" t="s">
+        <v>171</v>
+      </c>
+      <c r="E28" s="17" t="s">
+        <v>60</v>
       </c>
       <c r="F28" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="G28" s="19" t="s">
-        <v>172</v>
-      </c>
-      <c r="H28" s="20" t="s">
         <v>167</v>
       </c>
-      <c r="I28" s="27">
+      <c r="G28" s="25">
         <v>456.72</v>
       </c>
-      <c r="J28" s="21"/>
-      <c r="K28" s="21"/>
-      <c r="L28" s="16">
-        <v>4800</v>
-      </c>
-      <c r="M28" s="21">
-        <v>3</v>
-      </c>
-      <c r="N28" s="38"/>
-      <c r="O28" s="17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" ht="20.100000000000001" customHeight="1">
+      <c r="H28" s="19"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="15">
+        <v>4800</v>
+      </c>
+      <c r="K28" s="19">
+        <v>3</v>
+      </c>
+      <c r="L28" s="36"/>
+      <c r="M28" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="20.100000000000001" customHeight="1">
       <c r="A29" s="3">
         <v>26</v>
       </c>
-      <c r="B29" s="41" t="s">
+      <c r="B29" s="39" t="s">
         <v>106</v>
       </c>
-      <c r="C29" s="48"/>
-      <c r="D29" s="46" t="s">
-        <v>176</v>
-      </c>
-      <c r="E29" s="44" t="s">
-        <v>182</v>
+      <c r="C29" s="44"/>
+      <c r="D29" s="42" t="s">
+        <v>171</v>
+      </c>
+      <c r="E29" s="17" t="s">
+        <v>61</v>
       </c>
       <c r="F29" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="G29" s="19" t="s">
-        <v>172</v>
-      </c>
-      <c r="H29" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="I29" s="27">
+      <c r="G29" s="25">
         <v>265.76</v>
       </c>
-      <c r="J29" s="21"/>
-      <c r="K29" s="21"/>
-      <c r="L29" s="16">
-        <v>4800</v>
-      </c>
-      <c r="M29" s="21">
-        <v>3</v>
-      </c>
-      <c r="N29" s="38"/>
-      <c r="O29" s="17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" ht="20.100000000000001" customHeight="1">
+      <c r="H29" s="19"/>
+      <c r="I29" s="19"/>
+      <c r="J29" s="15">
+        <v>4800</v>
+      </c>
+      <c r="K29" s="19">
+        <v>3</v>
+      </c>
+      <c r="L29" s="36"/>
+      <c r="M29" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="20.100000000000001" customHeight="1">
       <c r="A30" s="3">
         <v>27</v>
       </c>
-      <c r="B30" s="41" t="s">
+      <c r="B30" s="39" t="s">
         <v>107</v>
       </c>
-      <c r="C30" s="48"/>
-      <c r="D30" s="46" t="s">
-        <v>176</v>
-      </c>
-      <c r="E30" s="44" t="s">
-        <v>182</v>
+      <c r="C30" s="44"/>
+      <c r="D30" s="42" t="s">
+        <v>171</v>
+      </c>
+      <c r="E30" s="17" t="s">
+        <v>62</v>
       </c>
       <c r="F30" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="G30" s="19" t="s">
-        <v>172</v>
-      </c>
-      <c r="H30" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="I30" s="27">
+      <c r="G30" s="25">
         <v>111.3</v>
       </c>
-      <c r="J30" s="21"/>
-      <c r="K30" s="21"/>
-      <c r="L30" s="16">
-        <v>4800</v>
-      </c>
-      <c r="M30" s="21">
-        <v>3</v>
-      </c>
-      <c r="N30" s="38"/>
-      <c r="O30" s="17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" ht="20.100000000000001" customHeight="1">
+      <c r="H30" s="19"/>
+      <c r="I30" s="19"/>
+      <c r="J30" s="15">
+        <v>4800</v>
+      </c>
+      <c r="K30" s="19">
+        <v>3</v>
+      </c>
+      <c r="L30" s="36"/>
+      <c r="M30" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="20.100000000000001" customHeight="1">
       <c r="A31" s="3">
         <v>28</v>
       </c>
-      <c r="B31" s="41" t="s">
+      <c r="B31" s="39" t="s">
         <v>108</v>
       </c>
-      <c r="C31" s="48"/>
-      <c r="D31" s="46" t="s">
-        <v>176</v>
-      </c>
-      <c r="E31" s="44" t="s">
-        <v>182</v>
+      <c r="C31" s="44"/>
+      <c r="D31" s="42" t="s">
+        <v>171</v>
+      </c>
+      <c r="E31" s="17" t="s">
+        <v>63</v>
       </c>
       <c r="F31" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="G31" s="19" t="s">
-        <v>172</v>
-      </c>
-      <c r="H31" s="20" t="s">
         <v>167</v>
       </c>
-      <c r="I31" s="27">
+      <c r="G31" s="25">
         <v>859.76</v>
       </c>
-      <c r="J31" s="21"/>
-      <c r="K31" s="21"/>
-      <c r="L31" s="16">
-        <v>4800</v>
-      </c>
-      <c r="M31" s="21">
-        <v>3</v>
-      </c>
-      <c r="N31" s="38"/>
-      <c r="O31" s="17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" ht="20.100000000000001" customHeight="1">
+      <c r="H31" s="19"/>
+      <c r="I31" s="19"/>
+      <c r="J31" s="15">
+        <v>4800</v>
+      </c>
+      <c r="K31" s="19">
+        <v>3</v>
+      </c>
+      <c r="L31" s="36"/>
+      <c r="M31" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" ht="20.100000000000001" customHeight="1">
       <c r="A32" s="3">
         <v>29</v>
       </c>
-      <c r="B32" s="42" t="s">
+      <c r="B32" s="40" t="s">
         <v>109</v>
       </c>
-      <c r="C32" s="48"/>
-      <c r="D32" s="46" t="s">
-        <v>180</v>
-      </c>
-      <c r="E32" s="44" t="s">
-        <v>182</v>
+      <c r="C32" s="44"/>
+      <c r="D32" s="42" t="s">
+        <v>174</v>
+      </c>
+      <c r="E32" s="17" t="s">
+        <v>64</v>
       </c>
       <c r="F32" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="G32" s="19" t="s">
-        <v>173</v>
-      </c>
-      <c r="H32" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="I32" s="27">
+      <c r="G32" s="25">
         <v>202.92</v>
       </c>
-      <c r="J32" s="21"/>
-      <c r="K32" s="21"/>
-      <c r="L32" s="16">
-        <v>4800</v>
-      </c>
-      <c r="M32" s="21">
-        <v>3</v>
-      </c>
-      <c r="N32" s="38"/>
-      <c r="O32" s="17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="33" spans="1:15" ht="20.100000000000001" customHeight="1">
+      <c r="H32" s="19"/>
+      <c r="I32" s="19"/>
+      <c r="J32" s="15">
+        <v>4800</v>
+      </c>
+      <c r="K32" s="19">
+        <v>3</v>
+      </c>
+      <c r="L32" s="36"/>
+      <c r="M32" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" ht="20.100000000000001" customHeight="1">
       <c r="A33" s="3">
         <v>30</v>
       </c>
-      <c r="B33" s="41" t="s">
+      <c r="B33" s="39" t="s">
         <v>110</v>
       </c>
-      <c r="C33" s="48"/>
-      <c r="D33" s="46" t="s">
-        <v>180</v>
-      </c>
-      <c r="E33" s="44" t="s">
-        <v>182</v>
+      <c r="C33" s="44"/>
+      <c r="D33" s="42" t="s">
+        <v>174</v>
+      </c>
+      <c r="E33" s="17" t="s">
+        <v>65</v>
       </c>
       <c r="F33" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="G33" s="19" t="s">
-        <v>173</v>
-      </c>
-      <c r="H33" s="20" t="s">
         <v>166</v>
       </c>
-      <c r="I33" s="27">
+      <c r="G33" s="25">
         <v>132</v>
       </c>
-      <c r="J33" s="21"/>
-      <c r="K33" s="21"/>
-      <c r="L33" s="16">
-        <v>4800</v>
-      </c>
-      <c r="M33" s="21">
-        <v>3</v>
-      </c>
-      <c r="N33" s="38"/>
-      <c r="O33" s="17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="34" spans="1:15" ht="20.100000000000001" customHeight="1">
+      <c r="H33" s="19"/>
+      <c r="I33" s="19"/>
+      <c r="J33" s="15">
+        <v>4800</v>
+      </c>
+      <c r="K33" s="19">
+        <v>3</v>
+      </c>
+      <c r="L33" s="36"/>
+      <c r="M33" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" ht="20.100000000000001" customHeight="1">
       <c r="A34" s="3">
         <v>31</v>
       </c>
-      <c r="B34" s="41" t="s">
+      <c r="B34" s="39" t="s">
         <v>111</v>
       </c>
-      <c r="C34" s="48"/>
-      <c r="D34" s="46" t="s">
-        <v>180</v>
-      </c>
-      <c r="E34" s="44" t="s">
-        <v>182</v>
+      <c r="C34" s="44"/>
+      <c r="D34" s="42" t="s">
+        <v>174</v>
+      </c>
+      <c r="E34" s="17" t="s">
+        <v>66</v>
       </c>
       <c r="F34" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="G34" s="19" t="s">
-        <v>173</v>
-      </c>
-      <c r="H34" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="I34" s="27">
+      <c r="G34" s="25">
         <v>118.8</v>
       </c>
-      <c r="J34" s="21"/>
-      <c r="K34" s="21"/>
-      <c r="L34" s="16">
-        <v>4800</v>
-      </c>
-      <c r="M34" s="21">
-        <v>3</v>
-      </c>
-      <c r="N34" s="38"/>
-      <c r="O34" s="17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15" ht="20.100000000000001" customHeight="1">
+      <c r="H34" s="19"/>
+      <c r="I34" s="19"/>
+      <c r="J34" s="15">
+        <v>4800</v>
+      </c>
+      <c r="K34" s="19">
+        <v>3</v>
+      </c>
+      <c r="L34" s="36"/>
+      <c r="M34" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" ht="20.100000000000001" customHeight="1">
       <c r="A35" s="3">
         <v>32</v>
       </c>
-      <c r="B35" s="41" t="s">
+      <c r="B35" s="39" t="s">
         <v>112</v>
       </c>
-      <c r="C35" s="48"/>
-      <c r="D35" s="46" t="s">
-        <v>180</v>
-      </c>
-      <c r="E35" s="44" t="s">
-        <v>182</v>
+      <c r="C35" s="44"/>
+      <c r="D35" s="42" t="s">
+        <v>174</v>
+      </c>
+      <c r="E35" s="17" t="s">
+        <v>67</v>
       </c>
       <c r="F35" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="G35" s="19" t="s">
-        <v>173</v>
-      </c>
-      <c r="H35" s="20" t="s">
         <v>166</v>
       </c>
-      <c r="I35" s="28">
+      <c r="G35" s="26">
         <v>1083.68</v>
       </c>
-      <c r="J35" s="21"/>
-      <c r="K35" s="21"/>
-      <c r="L35" s="16">
-        <v>4800</v>
-      </c>
-      <c r="M35" s="21">
-        <v>3</v>
-      </c>
-      <c r="N35" s="38"/>
-      <c r="O35" s="17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="36" spans="1:15" ht="20.100000000000001" customHeight="1">
+      <c r="H35" s="19"/>
+      <c r="I35" s="19"/>
+      <c r="J35" s="15">
+        <v>4800</v>
+      </c>
+      <c r="K35" s="19">
+        <v>3</v>
+      </c>
+      <c r="L35" s="36"/>
+      <c r="M35" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" ht="20.100000000000001" customHeight="1">
       <c r="A36" s="3">
         <v>33</v>
       </c>
-      <c r="B36" s="41" t="s">
+      <c r="B36" s="39" t="s">
         <v>113</v>
       </c>
-      <c r="C36" s="48"/>
-      <c r="D36" s="46" t="s">
-        <v>180</v>
-      </c>
-      <c r="E36" s="44" t="s">
-        <v>182</v>
+      <c r="C36" s="44"/>
+      <c r="D36" s="42" t="s">
+        <v>174</v>
+      </c>
+      <c r="E36" s="17" t="s">
+        <v>68</v>
       </c>
       <c r="F36" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="G36" s="19" t="s">
-        <v>173</v>
-      </c>
-      <c r="H36" s="20" t="s">
         <v>166</v>
       </c>
-      <c r="I36" s="27">
+      <c r="G36" s="25">
         <v>334.88</v>
       </c>
-      <c r="J36" s="21"/>
-      <c r="K36" s="21"/>
-      <c r="L36" s="16">
-        <v>4800</v>
-      </c>
-      <c r="M36" s="21">
-        <v>3</v>
-      </c>
-      <c r="N36" s="38"/>
-      <c r="O36" s="17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="37" spans="1:15" ht="20.100000000000001" customHeight="1">
+      <c r="H36" s="19"/>
+      <c r="I36" s="19"/>
+      <c r="J36" s="15">
+        <v>4800</v>
+      </c>
+      <c r="K36" s="19">
+        <v>3</v>
+      </c>
+      <c r="L36" s="36"/>
+      <c r="M36" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" ht="20.100000000000001" customHeight="1">
       <c r="A37" s="3">
         <v>34</v>
       </c>
-      <c r="B37" s="41" t="s">
+      <c r="B37" s="39" t="s">
         <v>114</v>
       </c>
-      <c r="C37" s="48"/>
-      <c r="D37" s="46" t="s">
-        <v>179</v>
-      </c>
-      <c r="E37" s="44" t="s">
-        <v>182</v>
+      <c r="C37" s="44"/>
+      <c r="D37" s="42" t="s">
+        <v>173</v>
+      </c>
+      <c r="E37" s="17" t="s">
+        <v>69</v>
       </c>
       <c r="F37" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="G37" s="19" t="s">
-        <v>183</v>
-      </c>
-      <c r="H37" s="20" t="s">
         <v>167</v>
       </c>
-      <c r="I37" s="27">
+      <c r="G37" s="25">
         <v>931.35</v>
       </c>
-      <c r="J37" s="21"/>
-      <c r="K37" s="21"/>
-      <c r="L37" s="16">
-        <v>4800</v>
-      </c>
-      <c r="M37" s="21">
-        <v>3</v>
-      </c>
-      <c r="N37" s="38"/>
-      <c r="O37" s="17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="38" spans="1:15" ht="20.100000000000001" customHeight="1">
+      <c r="H37" s="19"/>
+      <c r="I37" s="19"/>
+      <c r="J37" s="15">
+        <v>4800</v>
+      </c>
+      <c r="K37" s="19">
+        <v>3</v>
+      </c>
+      <c r="L37" s="36"/>
+      <c r="M37" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" ht="20.100000000000001" customHeight="1">
       <c r="A38" s="3">
         <v>35</v>
       </c>
-      <c r="B38" s="41" t="s">
+      <c r="B38" s="39" t="s">
         <v>115</v>
       </c>
-      <c r="C38" s="48"/>
-      <c r="D38" s="46" t="s">
-        <v>179</v>
-      </c>
-      <c r="E38" s="44" t="s">
-        <v>182</v>
+      <c r="C38" s="44"/>
+      <c r="D38" s="42" t="s">
+        <v>173</v>
+      </c>
+      <c r="E38" s="17" t="s">
+        <v>70</v>
       </c>
       <c r="F38" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="G38" s="19" t="s">
-        <v>183</v>
-      </c>
-      <c r="H38" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="I38" s="27">
+      <c r="G38" s="25">
         <v>329.88</v>
       </c>
-      <c r="J38" s="21"/>
-      <c r="K38" s="21"/>
-      <c r="L38" s="16">
-        <v>4800</v>
-      </c>
-      <c r="M38" s="21">
-        <v>3</v>
-      </c>
-      <c r="N38" s="38"/>
-      <c r="O38" s="17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="39" spans="1:15" ht="20.100000000000001" customHeight="1">
+      <c r="H38" s="19"/>
+      <c r="I38" s="19"/>
+      <c r="J38" s="15">
+        <v>4800</v>
+      </c>
+      <c r="K38" s="19">
+        <v>3</v>
+      </c>
+      <c r="L38" s="36"/>
+      <c r="M38" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" ht="20.100000000000001" customHeight="1">
       <c r="A39" s="3">
         <v>36</v>
       </c>
-      <c r="B39" s="41" t="s">
+      <c r="B39" s="39" t="s">
         <v>116</v>
       </c>
-      <c r="C39" s="48"/>
-      <c r="D39" s="46" t="s">
-        <v>179</v>
-      </c>
-      <c r="E39" s="44" t="s">
-        <v>182</v>
+      <c r="C39" s="44"/>
+      <c r="D39" s="42" t="s">
+        <v>173</v>
+      </c>
+      <c r="E39" s="17" t="s">
+        <v>85</v>
       </c>
       <c r="F39" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="G39" s="19" t="s">
-        <v>183</v>
-      </c>
-      <c r="H39" s="20" t="s">
         <v>165</v>
       </c>
-      <c r="I39" s="27">
+      <c r="G39" s="25">
         <v>282.39999999999998</v>
       </c>
-      <c r="J39" s="21"/>
-      <c r="K39" s="21"/>
-      <c r="L39" s="16">
-        <v>4800</v>
-      </c>
-      <c r="M39" s="21">
-        <v>3</v>
-      </c>
-      <c r="N39" s="38"/>
-      <c r="O39" s="17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="40" spans="1:15" ht="20.100000000000001" customHeight="1">
+      <c r="H39" s="19"/>
+      <c r="I39" s="19"/>
+      <c r="J39" s="15">
+        <v>4800</v>
+      </c>
+      <c r="K39" s="19">
+        <v>3</v>
+      </c>
+      <c r="L39" s="36"/>
+      <c r="M39" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" ht="20.100000000000001" customHeight="1">
       <c r="A40" s="3">
         <v>37</v>
       </c>
-      <c r="B40" s="41" t="s">
+      <c r="B40" s="39" t="s">
         <v>117</v>
       </c>
-      <c r="C40" s="48"/>
-      <c r="D40" s="46" t="s">
-        <v>179</v>
-      </c>
-      <c r="E40" s="44" t="s">
-        <v>182</v>
+      <c r="C40" s="44"/>
+      <c r="D40" s="42" t="s">
+        <v>173</v>
+      </c>
+      <c r="E40" s="17" t="s">
+        <v>86</v>
       </c>
       <c r="F40" s="18" t="s">
-        <v>86</v>
-      </c>
-      <c r="G40" s="19" t="s">
-        <v>184</v>
-      </c>
-      <c r="H40" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="I40" s="27">
+      <c r="G40" s="25">
         <v>64.8</v>
       </c>
-      <c r="J40" s="21"/>
-      <c r="K40" s="21"/>
-      <c r="L40" s="16">
-        <v>4800</v>
-      </c>
-      <c r="M40" s="21">
-        <v>3</v>
-      </c>
-      <c r="N40" s="38"/>
-      <c r="O40" s="17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="41" spans="1:15" ht="20.100000000000001" customHeight="1">
+      <c r="H40" s="19"/>
+      <c r="I40" s="19"/>
+      <c r="J40" s="15">
+        <v>4800</v>
+      </c>
+      <c r="K40" s="19">
+        <v>3</v>
+      </c>
+      <c r="L40" s="36"/>
+      <c r="M40" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" ht="20.100000000000001" customHeight="1">
       <c r="A41" s="3">
         <v>38</v>
       </c>
-      <c r="B41" s="41" t="s">
+      <c r="B41" s="39" t="s">
         <v>118</v>
       </c>
-      <c r="C41" s="48"/>
-      <c r="D41" s="46" t="s">
-        <v>179</v>
-      </c>
-      <c r="E41" s="44" t="s">
-        <v>182</v>
+      <c r="C41" s="44"/>
+      <c r="D41" s="42" t="s">
+        <v>173</v>
+      </c>
+      <c r="E41" s="17" t="s">
+        <v>87</v>
       </c>
       <c r="F41" s="18" t="s">
-        <v>87</v>
-      </c>
-      <c r="G41" s="19" t="s">
-        <v>184</v>
-      </c>
-      <c r="H41" s="20" t="s">
         <v>146</v>
       </c>
-      <c r="I41" s="27">
+      <c r="G41" s="25">
         <v>135.88</v>
       </c>
-      <c r="J41" s="21"/>
-      <c r="K41" s="21"/>
-      <c r="L41" s="16">
-        <v>4800</v>
-      </c>
-      <c r="M41" s="21">
-        <v>3</v>
-      </c>
-      <c r="N41" s="38"/>
-      <c r="O41" s="17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="42" spans="1:15" ht="20.100000000000001" customHeight="1">
+      <c r="H41" s="19"/>
+      <c r="I41" s="19"/>
+      <c r="J41" s="15">
+        <v>4800</v>
+      </c>
+      <c r="K41" s="19">
+        <v>3</v>
+      </c>
+      <c r="L41" s="36"/>
+      <c r="M41" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" ht="20.100000000000001" customHeight="1">
       <c r="A42" s="3">
         <v>39</v>
       </c>
-      <c r="B42" s="41" t="s">
+      <c r="B42" s="39" t="s">
         <v>79</v>
       </c>
-      <c r="C42" s="48"/>
-      <c r="D42" s="46" t="s">
-        <v>179</v>
-      </c>
-      <c r="E42" s="44" t="s">
-        <v>182</v>
+      <c r="C42" s="44"/>
+      <c r="D42" s="42" t="s">
+        <v>173</v>
+      </c>
+      <c r="E42" s="17" t="s">
+        <v>88</v>
       </c>
       <c r="F42" s="18" t="s">
-        <v>88</v>
-      </c>
-      <c r="G42" s="19" t="s">
-        <v>184</v>
-      </c>
-      <c r="H42" s="20" t="s">
         <v>167</v>
       </c>
-      <c r="I42" s="27">
+      <c r="G42" s="25">
         <v>64.8</v>
       </c>
-      <c r="J42" s="21"/>
-      <c r="K42" s="21"/>
-      <c r="L42" s="16">
-        <v>4800</v>
-      </c>
-      <c r="M42" s="21">
-        <v>3</v>
-      </c>
-      <c r="N42" s="38"/>
-      <c r="O42" s="17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="43" spans="1:15" ht="20.100000000000001" customHeight="1">
+      <c r="H42" s="19"/>
+      <c r="I42" s="19"/>
+      <c r="J42" s="15">
+        <v>4800</v>
+      </c>
+      <c r="K42" s="19">
+        <v>3</v>
+      </c>
+      <c r="L42" s="36"/>
+      <c r="M42" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" ht="20.100000000000001" customHeight="1">
       <c r="A43" s="3">
         <v>40</v>
       </c>
-      <c r="B43" s="41" t="s">
+      <c r="B43" s="39" t="s">
         <v>119</v>
       </c>
-      <c r="C43" s="48"/>
-      <c r="D43" s="46" t="s">
-        <v>179</v>
-      </c>
-      <c r="E43" s="44" t="s">
-        <v>182</v>
+      <c r="C43" s="44"/>
+      <c r="D43" s="42" t="s">
+        <v>173</v>
+      </c>
+      <c r="E43" s="17" t="s">
+        <v>89</v>
       </c>
       <c r="F43" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="G43" s="19" t="s">
-        <v>184</v>
-      </c>
-      <c r="H43" s="20" t="s">
         <v>165</v>
       </c>
-      <c r="I43" s="27">
+      <c r="G43" s="25">
         <v>609.76</v>
       </c>
-      <c r="J43" s="21"/>
-      <c r="K43" s="21"/>
-      <c r="L43" s="16">
-        <v>4800</v>
-      </c>
-      <c r="M43" s="21">
-        <v>3</v>
-      </c>
-      <c r="N43" s="38"/>
-      <c r="O43" s="17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="44" spans="1:15" ht="20.100000000000001" customHeight="1">
+      <c r="H43" s="19"/>
+      <c r="I43" s="19"/>
+      <c r="J43" s="15">
+        <v>4800</v>
+      </c>
+      <c r="K43" s="19">
+        <v>3</v>
+      </c>
+      <c r="L43" s="36"/>
+      <c r="M43" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" ht="20.100000000000001" customHeight="1">
       <c r="A44" s="3">
         <v>41</v>
       </c>
-      <c r="B44" s="41" t="s">
+      <c r="B44" s="39" t="s">
         <v>120</v>
       </c>
-      <c r="C44" s="48"/>
-      <c r="D44" s="46" t="s">
-        <v>179</v>
-      </c>
-      <c r="E44" s="44" t="s">
-        <v>182</v>
+      <c r="C44" s="44"/>
+      <c r="D44" s="42" t="s">
+        <v>173</v>
+      </c>
+      <c r="E44" s="17" t="s">
+        <v>90</v>
       </c>
       <c r="F44" s="18" t="s">
-        <v>90</v>
-      </c>
-      <c r="G44" s="19" t="s">
-        <v>184</v>
-      </c>
-      <c r="H44" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="I44" s="27">
+      <c r="G44" s="25">
         <v>602.96</v>
       </c>
-      <c r="J44" s="21"/>
-      <c r="K44" s="21"/>
-      <c r="L44" s="16">
-        <v>4800</v>
-      </c>
-      <c r="M44" s="21">
-        <v>3</v>
-      </c>
-      <c r="N44" s="38"/>
-      <c r="O44" s="17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="45" spans="1:15" ht="20.100000000000001" customHeight="1">
+      <c r="H44" s="19"/>
+      <c r="I44" s="19"/>
+      <c r="J44" s="15">
+        <v>4800</v>
+      </c>
+      <c r="K44" s="19">
+        <v>3</v>
+      </c>
+      <c r="L44" s="36"/>
+      <c r="M44" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" ht="20.100000000000001" customHeight="1">
       <c r="A45" s="3">
         <v>42</v>
       </c>
-      <c r="B45" s="41" t="s">
+      <c r="B45" s="39" t="s">
         <v>121</v>
       </c>
-      <c r="C45" s="48"/>
-      <c r="D45" s="46" t="s">
-        <v>179</v>
-      </c>
-      <c r="E45" s="44" t="s">
-        <v>182</v>
+      <c r="C45" s="44"/>
+      <c r="D45" s="42" t="s">
+        <v>173</v>
+      </c>
+      <c r="E45" s="17" t="s">
+        <v>91</v>
       </c>
       <c r="F45" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="G45" s="19" t="s">
-        <v>184</v>
-      </c>
-      <c r="H45" s="20" t="s">
-        <v>145</v>
-      </c>
-      <c r="I45" s="27">
+        <v>165</v>
+      </c>
+      <c r="G45" s="25">
         <v>59.84</v>
       </c>
-      <c r="J45" s="21"/>
-      <c r="K45" s="21"/>
-      <c r="L45" s="16">
-        <v>4800</v>
-      </c>
-      <c r="M45" s="21">
-        <v>3</v>
-      </c>
-      <c r="N45" s="38"/>
-      <c r="O45" s="17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="46" spans="1:15" ht="20.100000000000001" customHeight="1">
+      <c r="H45" s="19"/>
+      <c r="I45" s="19"/>
+      <c r="J45" s="15">
+        <v>4800</v>
+      </c>
+      <c r="K45" s="19">
+        <v>3</v>
+      </c>
+      <c r="L45" s="36"/>
+      <c r="M45" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" ht="20.100000000000001" customHeight="1">
       <c r="A46" s="3">
         <v>43</v>
       </c>
-      <c r="B46" s="41" t="s">
+      <c r="B46" s="39" t="s">
         <v>122</v>
       </c>
-      <c r="C46" s="48"/>
-      <c r="D46" s="46" t="s">
-        <v>179</v>
-      </c>
-      <c r="E46" s="44" t="s">
-        <v>182</v>
+      <c r="C46" s="44"/>
+      <c r="D46" s="42" t="s">
+        <v>173</v>
+      </c>
+      <c r="E46" s="17" t="s">
+        <v>92</v>
       </c>
       <c r="F46" s="18" t="s">
-        <v>92</v>
-      </c>
-      <c r="G46" s="19" t="s">
-        <v>184</v>
-      </c>
-      <c r="H46" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="I46" s="27">
+      <c r="G46" s="25">
         <v>90.8</v>
       </c>
-      <c r="J46" s="21"/>
-      <c r="K46" s="21"/>
-      <c r="L46" s="16">
-        <v>4800</v>
-      </c>
-      <c r="M46" s="21">
-        <v>3</v>
-      </c>
-      <c r="N46" s="38"/>
-      <c r="O46" s="17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="47" spans="1:15" ht="20.100000000000001" customHeight="1">
+      <c r="H46" s="19"/>
+      <c r="I46" s="19"/>
+      <c r="J46" s="15">
+        <v>4800</v>
+      </c>
+      <c r="K46" s="19">
+        <v>3</v>
+      </c>
+      <c r="L46" s="36"/>
+      <c r="M46" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" ht="20.100000000000001" customHeight="1">
       <c r="A47" s="3">
         <v>44</v>
       </c>
-      <c r="B47" s="41" t="s">
+      <c r="B47" s="39" t="s">
         <v>123</v>
       </c>
-      <c r="C47" s="48"/>
-      <c r="D47" s="46" t="s">
-        <v>179</v>
-      </c>
-      <c r="E47" s="44" t="s">
-        <v>182</v>
+      <c r="C47" s="44"/>
+      <c r="D47" s="42" t="s">
+        <v>173</v>
+      </c>
+      <c r="E47" s="17" t="s">
+        <v>93</v>
       </c>
       <c r="F47" s="18" t="s">
-        <v>93</v>
-      </c>
-      <c r="G47" s="19" t="s">
-        <v>184</v>
-      </c>
-      <c r="H47" s="20" t="s">
         <v>168</v>
       </c>
-      <c r="I47" s="27">
+      <c r="G47" s="25">
         <v>318.56</v>
       </c>
-      <c r="J47" s="21"/>
-      <c r="K47" s="21"/>
-      <c r="L47" s="16">
-        <v>4800</v>
-      </c>
-      <c r="M47" s="21">
-        <v>3</v>
-      </c>
-      <c r="N47" s="38"/>
-      <c r="O47" s="17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="48" spans="1:15" ht="20.100000000000001" customHeight="1">
+      <c r="H47" s="19"/>
+      <c r="I47" s="19"/>
+      <c r="J47" s="15">
+        <v>4800</v>
+      </c>
+      <c r="K47" s="19">
+        <v>3</v>
+      </c>
+      <c r="L47" s="36"/>
+      <c r="M47" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" ht="20.100000000000001" customHeight="1">
       <c r="A48" s="3">
         <v>45</v>
       </c>
-      <c r="B48" s="41" t="s">
+      <c r="B48" s="39" t="s">
         <v>124</v>
       </c>
-      <c r="C48" s="48"/>
-      <c r="D48" s="46" t="s">
-        <v>179</v>
-      </c>
-      <c r="E48" s="44" t="s">
-        <v>182</v>
+      <c r="C48" s="44"/>
+      <c r="D48" s="42" t="s">
+        <v>173</v>
+      </c>
+      <c r="E48" s="17" t="s">
+        <v>94</v>
       </c>
       <c r="F48" s="18" t="s">
-        <v>94</v>
-      </c>
-      <c r="G48" s="19" t="s">
-        <v>184</v>
-      </c>
-      <c r="H48" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="I48" s="27">
+      <c r="G48" s="25">
         <v>63</v>
       </c>
-      <c r="J48" s="21"/>
-      <c r="K48" s="21"/>
-      <c r="L48" s="16">
-        <v>4800</v>
-      </c>
-      <c r="M48" s="21">
-        <v>3</v>
-      </c>
-      <c r="N48" s="38"/>
-      <c r="O48" s="17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="49" spans="1:15" ht="20.100000000000001" customHeight="1">
+      <c r="H48" s="19"/>
+      <c r="I48" s="19"/>
+      <c r="J48" s="15">
+        <v>4800</v>
+      </c>
+      <c r="K48" s="19">
+        <v>3</v>
+      </c>
+      <c r="L48" s="36"/>
+      <c r="M48" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" ht="20.100000000000001" customHeight="1">
       <c r="A49" s="3">
         <v>46</v>
       </c>
-      <c r="B49" s="41" t="s">
+      <c r="B49" s="39" t="s">
         <v>81</v>
       </c>
-      <c r="C49" s="48"/>
-      <c r="D49" s="46" t="s">
-        <v>179</v>
-      </c>
-      <c r="E49" s="44" t="s">
-        <v>182</v>
+      <c r="C49" s="44"/>
+      <c r="D49" s="42" t="s">
+        <v>173</v>
+      </c>
+      <c r="E49" s="17" t="s">
+        <v>95</v>
       </c>
       <c r="F49" s="18" t="s">
-        <v>95</v>
-      </c>
-      <c r="G49" s="19" t="s">
-        <v>184</v>
-      </c>
-      <c r="H49" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="I49" s="27">
+      <c r="G49" s="25">
         <v>464.56</v>
       </c>
-      <c r="J49" s="21"/>
-      <c r="K49" s="21"/>
-      <c r="L49" s="16">
-        <v>4800</v>
-      </c>
-      <c r="M49" s="21">
-        <v>3</v>
-      </c>
-      <c r="N49" s="38"/>
-      <c r="O49" s="17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="50" spans="1:15" ht="20.100000000000001" customHeight="1">
+      <c r="H49" s="19"/>
+      <c r="I49" s="19"/>
+      <c r="J49" s="15">
+        <v>4800</v>
+      </c>
+      <c r="K49" s="19">
+        <v>3</v>
+      </c>
+      <c r="L49" s="36"/>
+      <c r="M49" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" ht="20.100000000000001" customHeight="1">
       <c r="A50" s="3">
         <v>47</v>
       </c>
-      <c r="B50" s="41" t="s">
+      <c r="B50" s="39" t="s">
         <v>82</v>
       </c>
-      <c r="C50" s="48"/>
-      <c r="D50" s="46" t="s">
-        <v>179</v>
-      </c>
-      <c r="E50" s="44" t="s">
-        <v>182</v>
+      <c r="C50" s="44"/>
+      <c r="D50" s="42" t="s">
+        <v>173</v>
+      </c>
+      <c r="E50" s="17" t="s">
+        <v>96</v>
       </c>
       <c r="F50" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="G50" s="19" t="s">
-        <v>184</v>
-      </c>
-      <c r="H50" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="I50" s="27">
+      <c r="G50" s="25">
         <v>126.36</v>
       </c>
-      <c r="J50" s="21"/>
-      <c r="K50" s="21"/>
-      <c r="L50" s="16">
-        <v>4800</v>
-      </c>
-      <c r="M50" s="21">
-        <v>3</v>
-      </c>
-      <c r="N50" s="38"/>
-      <c r="O50" s="17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="51" spans="1:15" ht="20.100000000000001" customHeight="1">
+      <c r="H50" s="19"/>
+      <c r="I50" s="19"/>
+      <c r="J50" s="15">
+        <v>4800</v>
+      </c>
+      <c r="K50" s="19">
+        <v>3</v>
+      </c>
+      <c r="L50" s="36"/>
+      <c r="M50" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" ht="20.100000000000001" customHeight="1">
       <c r="A51" s="3">
         <v>48</v>
       </c>
-      <c r="B51" s="41" t="s">
+      <c r="B51" s="39" t="s">
         <v>125</v>
       </c>
-      <c r="C51" s="48"/>
-      <c r="D51" s="46" t="s">
-        <v>179</v>
-      </c>
-      <c r="E51" s="44" t="s">
-        <v>182</v>
+      <c r="C51" s="44"/>
+      <c r="D51" s="42" t="s">
+        <v>173</v>
+      </c>
+      <c r="E51" s="17" t="s">
+        <v>97</v>
       </c>
       <c r="F51" s="18" t="s">
-        <v>97</v>
-      </c>
-      <c r="G51" s="19" t="s">
-        <v>184</v>
-      </c>
-      <c r="H51" s="20" t="s">
         <v>165</v>
       </c>
-      <c r="I51" s="27">
+      <c r="G51" s="25">
         <v>148.52000000000001</v>
       </c>
-      <c r="J51" s="21"/>
-      <c r="K51" s="21"/>
-      <c r="L51" s="16">
-        <v>4800</v>
-      </c>
-      <c r="M51" s="21">
-        <v>3</v>
-      </c>
-      <c r="N51" s="38"/>
-      <c r="O51" s="17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="52" spans="1:15" ht="20.100000000000001" customHeight="1">
+      <c r="H51" s="19"/>
+      <c r="I51" s="19"/>
+      <c r="J51" s="15">
+        <v>4800</v>
+      </c>
+      <c r="K51" s="19">
+        <v>3</v>
+      </c>
+      <c r="L51" s="36"/>
+      <c r="M51" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" ht="20.100000000000001" customHeight="1">
       <c r="A52" s="3">
         <v>49</v>
       </c>
-      <c r="B52" s="41" t="s">
+      <c r="B52" s="39" t="s">
         <v>126</v>
       </c>
-      <c r="C52" s="48"/>
-      <c r="D52" s="46" t="s">
-        <v>179</v>
-      </c>
-      <c r="E52" s="44" t="s">
-        <v>182</v>
+      <c r="C52" s="44"/>
+      <c r="D52" s="42" t="s">
+        <v>173</v>
+      </c>
+      <c r="E52" s="17" t="s">
+        <v>98</v>
       </c>
       <c r="F52" s="18" t="s">
-        <v>98</v>
-      </c>
-      <c r="G52" s="19" t="s">
-        <v>184</v>
-      </c>
-      <c r="H52" s="20" t="s">
         <v>166</v>
       </c>
-      <c r="I52" s="27">
+      <c r="G52" s="25">
         <v>511.44</v>
       </c>
-      <c r="J52" s="21"/>
-      <c r="K52" s="21"/>
-      <c r="L52" s="16">
-        <v>4800</v>
-      </c>
-      <c r="M52" s="21">
-        <v>3</v>
-      </c>
-      <c r="N52" s="38"/>
-      <c r="O52" s="17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="53" spans="1:15" ht="20.100000000000001" customHeight="1">
+      <c r="H52" s="19"/>
+      <c r="I52" s="19"/>
+      <c r="J52" s="15">
+        <v>4800</v>
+      </c>
+      <c r="K52" s="19">
+        <v>3</v>
+      </c>
+      <c r="L52" s="36"/>
+      <c r="M52" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" ht="20.100000000000001" customHeight="1">
       <c r="A53" s="3">
         <v>50</v>
       </c>
-      <c r="B53" s="41" t="s">
+      <c r="B53" s="39" t="s">
         <v>127</v>
       </c>
-      <c r="C53" s="48"/>
-      <c r="D53" s="46" t="s">
-        <v>179</v>
-      </c>
-      <c r="E53" s="44" t="s">
-        <v>182</v>
+      <c r="C53" s="44"/>
+      <c r="D53" s="42" t="s">
+        <v>173</v>
+      </c>
+      <c r="E53" s="17" t="s">
+        <v>99</v>
       </c>
       <c r="F53" s="18" t="s">
-        <v>99</v>
-      </c>
-      <c r="G53" s="19" t="s">
-        <v>184</v>
-      </c>
-      <c r="H53" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="I53" s="27">
+      <c r="G53" s="25">
         <v>31.5</v>
       </c>
-      <c r="J53" s="21"/>
-      <c r="K53" s="21"/>
-      <c r="L53" s="16">
-        <v>4800</v>
-      </c>
-      <c r="M53" s="21">
-        <v>3</v>
-      </c>
-      <c r="N53" s="38"/>
-      <c r="O53" s="17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="54" spans="1:15" ht="20.100000000000001" customHeight="1">
+      <c r="H53" s="19"/>
+      <c r="I53" s="19"/>
+      <c r="J53" s="15">
+        <v>4800</v>
+      </c>
+      <c r="K53" s="19">
+        <v>3</v>
+      </c>
+      <c r="L53" s="36"/>
+      <c r="M53" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" ht="20.100000000000001" customHeight="1">
       <c r="A54" s="3">
         <v>51</v>
       </c>
-      <c r="B54" s="41" t="s">
+      <c r="B54" s="39" t="s">
         <v>76</v>
       </c>
-      <c r="C54" s="48"/>
-      <c r="D54" s="46" t="s">
-        <v>179</v>
-      </c>
-      <c r="E54" s="44" t="s">
-        <v>182</v>
+      <c r="C54" s="44"/>
+      <c r="D54" s="42" t="s">
+        <v>173</v>
+      </c>
+      <c r="E54" s="17" t="s">
+        <v>133</v>
       </c>
       <c r="F54" s="18" t="s">
-        <v>133</v>
-      </c>
-      <c r="G54" s="19" t="s">
-        <v>184</v>
-      </c>
-      <c r="H54" s="20" t="s">
         <v>167</v>
       </c>
-      <c r="I54" s="27">
+      <c r="G54" s="25">
         <v>60.96</v>
       </c>
-      <c r="J54" s="21"/>
-      <c r="K54" s="21"/>
-      <c r="L54" s="16">
-        <v>4800</v>
-      </c>
-      <c r="M54" s="21">
-        <v>3</v>
-      </c>
-      <c r="N54" s="38"/>
-      <c r="O54" s="17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="55" spans="1:15" ht="20.100000000000001" customHeight="1">
+      <c r="H54" s="19"/>
+      <c r="I54" s="19"/>
+      <c r="J54" s="15">
+        <v>4800</v>
+      </c>
+      <c r="K54" s="19">
+        <v>3</v>
+      </c>
+      <c r="L54" s="36"/>
+      <c r="M54" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" ht="20.100000000000001" customHeight="1">
       <c r="A55" s="3">
         <v>52</v>
       </c>
-      <c r="B55" s="41" t="s">
+      <c r="B55" s="39" t="s">
         <v>128</v>
       </c>
-      <c r="C55" s="48"/>
-      <c r="D55" s="46" t="s">
-        <v>179</v>
-      </c>
-      <c r="E55" s="44" t="s">
-        <v>182</v>
+      <c r="C55" s="44"/>
+      <c r="D55" s="42" t="s">
+        <v>173</v>
+      </c>
+      <c r="E55" s="17" t="s">
+        <v>134</v>
       </c>
       <c r="F55" s="18" t="s">
-        <v>134</v>
-      </c>
-      <c r="G55" s="19" t="s">
-        <v>184</v>
-      </c>
-      <c r="H55" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="I55" s="27">
+      <c r="G55" s="25">
         <v>826.56</v>
       </c>
-      <c r="J55" s="21"/>
-      <c r="K55" s="21"/>
-      <c r="L55" s="16">
-        <v>4800</v>
-      </c>
-      <c r="M55" s="21">
-        <v>3</v>
-      </c>
-      <c r="N55" s="38"/>
-      <c r="O55" s="17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="56" spans="1:15" ht="20.100000000000001" customHeight="1">
+      <c r="H55" s="19"/>
+      <c r="I55" s="19"/>
+      <c r="J55" s="15">
+        <v>4800</v>
+      </c>
+      <c r="K55" s="19">
+        <v>3</v>
+      </c>
+      <c r="L55" s="36"/>
+      <c r="M55" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" ht="20.100000000000001" customHeight="1">
       <c r="A56" s="3">
         <v>53</v>
       </c>
-      <c r="B56" s="41" t="s">
+      <c r="B56" s="39" t="s">
         <v>77</v>
       </c>
-      <c r="C56" s="48"/>
-      <c r="D56" s="46" t="s">
-        <v>179</v>
-      </c>
-      <c r="E56" s="44" t="s">
-        <v>182</v>
+      <c r="C56" s="44"/>
+      <c r="D56" s="42" t="s">
+        <v>173</v>
+      </c>
+      <c r="E56" s="17" t="s">
+        <v>135</v>
       </c>
       <c r="F56" s="18" t="s">
-        <v>135</v>
-      </c>
-      <c r="G56" s="19" t="s">
-        <v>184</v>
-      </c>
-      <c r="H56" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="I56" s="27">
+      <c r="G56" s="25">
         <v>127.8</v>
       </c>
-      <c r="J56" s="21"/>
-      <c r="K56" s="21"/>
-      <c r="L56" s="16">
-        <v>4800</v>
-      </c>
-      <c r="M56" s="21">
-        <v>3</v>
-      </c>
-      <c r="N56" s="38"/>
-      <c r="O56" s="17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="57" spans="1:15" ht="20.100000000000001" customHeight="1">
+      <c r="H56" s="19"/>
+      <c r="I56" s="19"/>
+      <c r="J56" s="15">
+        <v>4800</v>
+      </c>
+      <c r="K56" s="19">
+        <v>3</v>
+      </c>
+      <c r="L56" s="36"/>
+      <c r="M56" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" ht="20.100000000000001" customHeight="1">
       <c r="A57" s="3">
         <v>54</v>
       </c>
-      <c r="B57" s="41" t="s">
+      <c r="B57" s="39" t="s">
         <v>129</v>
       </c>
-      <c r="C57" s="48"/>
-      <c r="D57" s="46" t="s">
-        <v>179</v>
-      </c>
-      <c r="E57" s="44" t="s">
-        <v>182</v>
+      <c r="C57" s="44"/>
+      <c r="D57" s="42" t="s">
+        <v>173</v>
+      </c>
+      <c r="E57" s="17" t="s">
+        <v>136</v>
       </c>
       <c r="F57" s="18" t="s">
-        <v>136</v>
-      </c>
-      <c r="G57" s="19" t="s">
-        <v>184</v>
-      </c>
-      <c r="H57" s="20" t="s">
         <v>146</v>
       </c>
-      <c r="I57" s="27">
+      <c r="G57" s="25">
         <v>202.4</v>
       </c>
-      <c r="J57" s="21"/>
-      <c r="K57" s="21"/>
-      <c r="L57" s="16">
-        <v>4800</v>
-      </c>
-      <c r="M57" s="21">
-        <v>3</v>
-      </c>
-      <c r="N57" s="38"/>
-      <c r="O57" s="17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="58" spans="1:15" ht="20.100000000000001" customHeight="1">
+      <c r="H57" s="19"/>
+      <c r="I57" s="19"/>
+      <c r="J57" s="15">
+        <v>4800</v>
+      </c>
+      <c r="K57" s="19">
+        <v>3</v>
+      </c>
+      <c r="L57" s="36"/>
+      <c r="M57" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" ht="20.100000000000001" customHeight="1">
       <c r="A58" s="3">
         <v>55</v>
       </c>
-      <c r="B58" s="41" t="s">
+      <c r="B58" s="39" t="s">
         <v>130</v>
       </c>
-      <c r="C58" s="48"/>
-      <c r="D58" s="46" t="s">
-        <v>179</v>
-      </c>
-      <c r="E58" s="44" t="s">
-        <v>182</v>
+      <c r="C58" s="44"/>
+      <c r="D58" s="42" t="s">
+        <v>173</v>
+      </c>
+      <c r="E58" s="17" t="s">
+        <v>137</v>
       </c>
       <c r="F58" s="18" t="s">
-        <v>137</v>
-      </c>
-      <c r="G58" s="19" t="s">
-        <v>184</v>
-      </c>
-      <c r="H58" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="I58" s="27">
+      <c r="G58" s="25">
         <v>257.31</v>
       </c>
-      <c r="J58" s="21"/>
-      <c r="K58" s="21"/>
-      <c r="L58" s="16">
-        <v>4800</v>
-      </c>
-      <c r="M58" s="21">
-        <v>3</v>
-      </c>
-      <c r="N58" s="38"/>
-      <c r="O58" s="17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="59" spans="1:15" ht="20.100000000000001" customHeight="1">
+      <c r="H58" s="19"/>
+      <c r="I58" s="19"/>
+      <c r="J58" s="15">
+        <v>4800</v>
+      </c>
+      <c r="K58" s="19">
+        <v>3</v>
+      </c>
+      <c r="L58" s="36"/>
+      <c r="M58" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" ht="20.100000000000001" customHeight="1">
       <c r="A59" s="3">
         <v>56</v>
       </c>
-      <c r="B59" s="41" t="s">
+      <c r="B59" s="39" t="s">
         <v>131</v>
       </c>
-      <c r="C59" s="48"/>
-      <c r="D59" s="46" t="s">
-        <v>179</v>
-      </c>
-      <c r="E59" s="44" t="s">
-        <v>182</v>
+      <c r="C59" s="44"/>
+      <c r="D59" s="42" t="s">
+        <v>173</v>
+      </c>
+      <c r="E59" s="17" t="s">
+        <v>138</v>
       </c>
       <c r="F59" s="18" t="s">
-        <v>138</v>
-      </c>
-      <c r="G59" s="19" t="s">
-        <v>184</v>
-      </c>
-      <c r="H59" s="20" t="s">
-        <v>145</v>
-      </c>
-      <c r="I59" s="28">
+        <v>168</v>
+      </c>
+      <c r="G59" s="26">
         <v>1143.71</v>
       </c>
-      <c r="J59" s="21"/>
-      <c r="K59" s="21"/>
-      <c r="L59" s="16">
-        <v>4800</v>
-      </c>
-      <c r="M59" s="21">
-        <v>3</v>
-      </c>
-      <c r="N59" s="38"/>
-      <c r="O59" s="17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="60" spans="1:15" ht="20.100000000000001" customHeight="1">
+      <c r="H59" s="19"/>
+      <c r="I59" s="19"/>
+      <c r="J59" s="15">
+        <v>4800</v>
+      </c>
+      <c r="K59" s="19">
+        <v>3</v>
+      </c>
+      <c r="L59" s="36"/>
+      <c r="M59" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" ht="20.100000000000001" customHeight="1">
       <c r="A60" s="3">
         <v>57</v>
       </c>
-      <c r="B60" s="41" t="s">
+      <c r="B60" s="39" t="s">
         <v>132</v>
       </c>
-      <c r="C60" s="49"/>
-      <c r="D60" s="46" t="s">
-        <v>179</v>
-      </c>
-      <c r="E60" s="44" t="s">
-        <v>182</v>
+      <c r="C60" s="45"/>
+      <c r="D60" s="42" t="s">
+        <v>173</v>
+      </c>
+      <c r="E60" s="17" t="s">
+        <v>139</v>
       </c>
       <c r="F60" s="18" t="s">
-        <v>139</v>
-      </c>
-      <c r="G60" s="19" t="s">
-        <v>184</v>
-      </c>
-      <c r="H60" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="I60" s="27">
+      <c r="G60" s="25">
         <v>31.5</v>
       </c>
-      <c r="J60" s="21"/>
-      <c r="K60" s="21"/>
-      <c r="L60" s="16">
-        <v>4800</v>
-      </c>
-      <c r="M60" s="21">
-        <v>3</v>
-      </c>
-      <c r="N60" s="38"/>
-      <c r="O60" s="17" t="s">
+      <c r="H60" s="19"/>
+      <c r="I60" s="19"/>
+      <c r="J60" s="15">
+        <v>4800</v>
+      </c>
+      <c r="K60" s="19">
+        <v>3</v>
+      </c>
+      <c r="L60" s="36"/>
+      <c r="M60" s="16" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="F1:F60" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <mergeCells count="6">
     <mergeCell ref="C23:C60"/>
-    <mergeCell ref="O2:Q2"/>
-    <mergeCell ref="A2:N2"/>
-    <mergeCell ref="A1:Q1"/>
+    <mergeCell ref="M2:O2"/>
+    <mergeCell ref="A2:L2"/>
+    <mergeCell ref="A1:O1"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:C22"/>
   </mergeCells>
@@ -4989,90 +4568,90 @@
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2"/>
   <sheetData>
     <row r="1" spans="1:2" ht="13.8">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="32" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="13.8">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="33" t="s">
         <v>145</v>
       </c>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="33" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="13.8">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="33" t="s">
         <v>146</v>
       </c>
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="33" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="13.8">
-      <c r="A4" s="35" t="s">
+      <c r="A4" s="33" t="s">
         <v>147</v>
       </c>
-      <c r="B4" s="35" t="s">
+      <c r="B4" s="33" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="13.8">
-      <c r="A5" s="35" t="s">
+      <c r="A5" s="33" t="s">
         <v>148</v>
       </c>
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="33" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="13.8">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="33" t="s">
         <v>149</v>
       </c>
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="33" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="13.8">
-      <c r="A7" s="35" t="s">
+      <c r="A7" s="33" t="s">
         <v>150</v>
       </c>
-      <c r="B7" s="35" t="s">
+      <c r="B7" s="33" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="13.8">
-      <c r="A8" s="35" t="s">
+      <c r="A8" s="33" t="s">
         <v>151</v>
       </c>
-      <c r="B8" s="35" t="s">
+      <c r="B8" s="33" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="13.8">
-      <c r="A9" s="35" t="s">
+      <c r="A9" s="33" t="s">
         <v>152</v>
       </c>
-      <c r="B9" s="35" t="s">
+      <c r="B9" s="33" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="13.8">
-      <c r="A10" s="35" t="s">
+      <c r="A10" s="33" t="s">
         <v>153</v>
       </c>
-      <c r="B10" s="35" t="s">
+      <c r="B10" s="33" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="13.8">
-      <c r="A11" s="35" t="s">
+      <c r="A11" s="33" t="s">
         <v>154</v>
       </c>
-      <c r="B11" s="35" t="s">
+      <c r="B11" s="33" t="s">
         <v>163</v>
       </c>
     </row>
@@ -5120,7 +4699,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="17.25" customHeight="1">
-      <c r="A2" s="59">
+      <c r="A2" s="55">
         <v>1</v>
       </c>
       <c r="B2" s="5">
@@ -5143,7 +4722,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A3" s="59"/>
+      <c r="A3" s="55"/>
       <c r="B3" s="5">
         <v>1</v>
       </c>
@@ -5164,7 +4743,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="17.25" customHeight="1">
-      <c r="A4" s="59"/>
+      <c r="A4" s="55"/>
       <c r="B4" s="5">
         <v>1</v>
       </c>
@@ -5208,7 +4787,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="13.8">
-      <c r="A6" s="59">
+      <c r="A6" s="55">
         <v>3</v>
       </c>
       <c r="B6" s="5">
@@ -5231,7 +4810,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="13.8">
-      <c r="A7" s="59"/>
+      <c r="A7" s="55"/>
       <c r="B7" s="5">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
by saw -permutation -done
</commit_message>
<xml_diff>
--- a/DataSource/InputData.xlsx
+++ b/DataSource/InputData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Job\Wyzrs\Dev3\Project\DEV-3_Nevron_0601\DEV-3_Nevron_0601\DEV-3_Nevron_0601\DEV-3_Nevron_0429\DEV-3_Nevron\DataSource\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Job\Wyzrs\Dev3\Project\DEV-3_Nevron_FINAL\DEV-3_Nevron_0601\DEV-3_Nevron_0601\DEV-3_Nevron_0429\DEV-3_Nevron\DataSource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D77B46FF-34E0-4CCC-BD2C-03CE1E0CEEAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3C83272-6784-4AC3-898C-DAF5DBACA614}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2075,7 +2075,7 @@
       <pane xSplit="4" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="L5" sqref="L5"/>
+      <selection pane="bottomRight" activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="20.100000000000001" customHeight="1"/>

</xml_diff>